<commit_message>
Remove consolidated documentation files - all content merged into README.md
</commit_message>
<xml_diff>
--- a/data/Trip Summary.xlsx
+++ b/data/Trip Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T201"/>
+  <dimension ref="A1:AH205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,76 @@
           <t>recommendation_ar</t>
         </is>
       </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>task_completed</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>completion_date</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>points_earned</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>driver_name</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>traffic_congestion_km</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>weather_condition</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>traffic_violations</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>accidents_count</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>phone_usage</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>road_quality</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>trip_duration</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>distance_driven</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>night_driving_hours</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_passengers</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -618,6 +688,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -702,6 +786,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -786,6 +884,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -870,6 +982,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -954,6 +1080,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1038,6 +1178,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1122,6 +1276,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1206,6 +1374,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1290,6 +1472,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1374,6 +1570,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1458,6 +1668,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1542,6 +1766,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1626,6 +1864,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1710,6 +1962,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1794,6 +2060,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1878,6 +2158,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1962,6 +2256,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2046,6 +2354,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2130,6 +2452,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+      <c r="AC20" t="inlineStr"/>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2214,6 +2550,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2298,6 +2648,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2382,6 +2746,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2466,6 +2844,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr"/>
+      <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2550,6 +2942,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr"/>
+      <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2634,6 +3040,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
+      <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2718,6 +3138,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2802,6 +3236,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2886,6 +3334,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2970,6 +3432,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr"/>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3054,6 +3530,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3138,6 +3628,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3222,6 +3726,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3306,6 +3824,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
+      <c r="AB34" t="inlineStr"/>
+      <c r="AC34" t="inlineStr"/>
+      <c r="AD34" t="inlineStr"/>
+      <c r="AE34" t="inlineStr"/>
+      <c r="AF34" t="inlineStr"/>
+      <c r="AG34" t="inlineStr"/>
+      <c r="AH34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3390,6 +3922,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr"/>
+      <c r="AB35" t="inlineStr"/>
+      <c r="AC35" t="inlineStr"/>
+      <c r="AD35" t="inlineStr"/>
+      <c r="AE35" t="inlineStr"/>
+      <c r="AF35" t="inlineStr"/>
+      <c r="AG35" t="inlineStr"/>
+      <c r="AH35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3474,6 +4020,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr"/>
+      <c r="Z36" t="inlineStr"/>
+      <c r="AA36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr"/>
+      <c r="AC36" t="inlineStr"/>
+      <c r="AD36" t="inlineStr"/>
+      <c r="AE36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr"/>
+      <c r="AG36" t="inlineStr"/>
+      <c r="AH36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3558,6 +4118,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="inlineStr"/>
+      <c r="Z37" t="inlineStr"/>
+      <c r="AA37" t="inlineStr"/>
+      <c r="AB37" t="inlineStr"/>
+      <c r="AC37" t="inlineStr"/>
+      <c r="AD37" t="inlineStr"/>
+      <c r="AE37" t="inlineStr"/>
+      <c r="AF37" t="inlineStr"/>
+      <c r="AG37" t="inlineStr"/>
+      <c r="AH37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3642,6 +4216,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr"/>
+      <c r="Z38" t="inlineStr"/>
+      <c r="AA38" t="inlineStr"/>
+      <c r="AB38" t="inlineStr"/>
+      <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="inlineStr"/>
+      <c r="AE38" t="inlineStr"/>
+      <c r="AF38" t="inlineStr"/>
+      <c r="AG38" t="inlineStr"/>
+      <c r="AH38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3726,6 +4314,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr"/>
+      <c r="Z39" t="inlineStr"/>
+      <c r="AA39" t="inlineStr"/>
+      <c r="AB39" t="inlineStr"/>
+      <c r="AC39" t="inlineStr"/>
+      <c r="AD39" t="inlineStr"/>
+      <c r="AE39" t="inlineStr"/>
+      <c r="AF39" t="inlineStr"/>
+      <c r="AG39" t="inlineStr"/>
+      <c r="AH39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3810,6 +4412,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr"/>
+      <c r="Z40" t="inlineStr"/>
+      <c r="AA40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr"/>
+      <c r="AC40" t="inlineStr"/>
+      <c r="AD40" t="inlineStr"/>
+      <c r="AE40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="inlineStr"/>
+      <c r="AH40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3894,6 +4510,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="inlineStr"/>
+      <c r="AA41" t="inlineStr"/>
+      <c r="AB41" t="inlineStr"/>
+      <c r="AC41" t="inlineStr"/>
+      <c r="AD41" t="inlineStr"/>
+      <c r="AE41" t="inlineStr"/>
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="inlineStr"/>
+      <c r="AH41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3978,6 +4608,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr"/>
+      <c r="Z42" t="inlineStr"/>
+      <c r="AA42" t="inlineStr"/>
+      <c r="AB42" t="inlineStr"/>
+      <c r="AC42" t="inlineStr"/>
+      <c r="AD42" t="inlineStr"/>
+      <c r="AE42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr"/>
+      <c r="AG42" t="inlineStr"/>
+      <c r="AH42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4062,6 +4706,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
+      <c r="Z43" t="inlineStr"/>
+      <c r="AA43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr"/>
+      <c r="AC43" t="inlineStr"/>
+      <c r="AD43" t="inlineStr"/>
+      <c r="AE43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr"/>
+      <c r="AG43" t="inlineStr"/>
+      <c r="AH43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4146,6 +4804,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
+      <c r="Y44" t="inlineStr"/>
+      <c r="Z44" t="inlineStr"/>
+      <c r="AA44" t="inlineStr"/>
+      <c r="AB44" t="inlineStr"/>
+      <c r="AC44" t="inlineStr"/>
+      <c r="AD44" t="inlineStr"/>
+      <c r="AE44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr"/>
+      <c r="AG44" t="inlineStr"/>
+      <c r="AH44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4230,6 +4902,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr"/>
+      <c r="Z45" t="inlineStr"/>
+      <c r="AA45" t="inlineStr"/>
+      <c r="AB45" t="inlineStr"/>
+      <c r="AC45" t="inlineStr"/>
+      <c r="AD45" t="inlineStr"/>
+      <c r="AE45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr"/>
+      <c r="AG45" t="inlineStr"/>
+      <c r="AH45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4314,6 +5000,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="inlineStr"/>
+      <c r="AA46" t="inlineStr"/>
+      <c r="AB46" t="inlineStr"/>
+      <c r="AC46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr"/>
+      <c r="AE46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr"/>
+      <c r="AG46" t="inlineStr"/>
+      <c r="AH46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4398,6 +5098,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr"/>
+      <c r="Z47" t="inlineStr"/>
+      <c r="AA47" t="inlineStr"/>
+      <c r="AB47" t="inlineStr"/>
+      <c r="AC47" t="inlineStr"/>
+      <c r="AD47" t="inlineStr"/>
+      <c r="AE47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr"/>
+      <c r="AG47" t="inlineStr"/>
+      <c r="AH47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4482,6 +5196,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr"/>
+      <c r="Z48" t="inlineStr"/>
+      <c r="AA48" t="inlineStr"/>
+      <c r="AB48" t="inlineStr"/>
+      <c r="AC48" t="inlineStr"/>
+      <c r="AD48" t="inlineStr"/>
+      <c r="AE48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="inlineStr"/>
+      <c r="AH48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4566,6 +5294,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr"/>
+      <c r="Z49" t="inlineStr"/>
+      <c r="AA49" t="inlineStr"/>
+      <c r="AB49" t="inlineStr"/>
+      <c r="AC49" t="inlineStr"/>
+      <c r="AD49" t="inlineStr"/>
+      <c r="AE49" t="inlineStr"/>
+      <c r="AF49" t="inlineStr"/>
+      <c r="AG49" t="inlineStr"/>
+      <c r="AH49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4650,6 +5392,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
+      <c r="Z50" t="inlineStr"/>
+      <c r="AA50" t="inlineStr"/>
+      <c r="AB50" t="inlineStr"/>
+      <c r="AC50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr"/>
+      <c r="AH50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4734,6 +5490,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
+      <c r="Z51" t="inlineStr"/>
+      <c r="AA51" t="inlineStr"/>
+      <c r="AB51" t="inlineStr"/>
+      <c r="AC51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr"/>
+      <c r="AE51" t="inlineStr"/>
+      <c r="AF51" t="inlineStr"/>
+      <c r="AG51" t="inlineStr"/>
+      <c r="AH51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4818,6 +5588,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
+      <c r="Z52" t="inlineStr"/>
+      <c r="AA52" t="inlineStr"/>
+      <c r="AB52" t="inlineStr"/>
+      <c r="AC52" t="inlineStr"/>
+      <c r="AD52" t="inlineStr"/>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4902,6 +5686,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="inlineStr"/>
+      <c r="Z53" t="inlineStr"/>
+      <c r="AA53" t="inlineStr"/>
+      <c r="AB53" t="inlineStr"/>
+      <c r="AC53" t="inlineStr"/>
+      <c r="AD53" t="inlineStr"/>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr"/>
+      <c r="AH53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4986,6 +5784,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
+      <c r="AB54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -5070,6 +5882,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
+      <c r="AA55" t="inlineStr"/>
+      <c r="AB55" t="inlineStr"/>
+      <c r="AC55" t="inlineStr"/>
+      <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -5154,6 +5980,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
+      <c r="AA56" t="inlineStr"/>
+      <c r="AB56" t="inlineStr"/>
+      <c r="AC56" t="inlineStr"/>
+      <c r="AD56" t="inlineStr"/>
+      <c r="AE56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5238,6 +6078,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
+      <c r="AA57" t="inlineStr"/>
+      <c r="AB57" t="inlineStr"/>
+      <c r="AC57" t="inlineStr"/>
+      <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -5322,6 +6176,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr"/>
+      <c r="Z58" t="inlineStr"/>
+      <c r="AA58" t="inlineStr"/>
+      <c r="AB58" t="inlineStr"/>
+      <c r="AC58" t="inlineStr"/>
+      <c r="AD58" t="inlineStr"/>
+      <c r="AE58" t="inlineStr"/>
+      <c r="AF58" t="inlineStr"/>
+      <c r="AG58" t="inlineStr"/>
+      <c r="AH58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5406,6 +6274,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+      <c r="Y59" t="inlineStr"/>
+      <c r="Z59" t="inlineStr"/>
+      <c r="AA59" t="inlineStr"/>
+      <c r="AB59" t="inlineStr"/>
+      <c r="AC59" t="inlineStr"/>
+      <c r="AD59" t="inlineStr"/>
+      <c r="AE59" t="inlineStr"/>
+      <c r="AF59" t="inlineStr"/>
+      <c r="AG59" t="inlineStr"/>
+      <c r="AH59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5490,6 +6372,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+      <c r="Y60" t="inlineStr"/>
+      <c r="Z60" t="inlineStr"/>
+      <c r="AA60" t="inlineStr"/>
+      <c r="AB60" t="inlineStr"/>
+      <c r="AC60" t="inlineStr"/>
+      <c r="AD60" t="inlineStr"/>
+      <c r="AE60" t="inlineStr"/>
+      <c r="AF60" t="inlineStr"/>
+      <c r="AG60" t="inlineStr"/>
+      <c r="AH60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5574,6 +6470,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
+      <c r="Z61" t="inlineStr"/>
+      <c r="AA61" t="inlineStr"/>
+      <c r="AB61" t="inlineStr"/>
+      <c r="AC61" t="inlineStr"/>
+      <c r="AD61" t="inlineStr"/>
+      <c r="AE61" t="inlineStr"/>
+      <c r="AF61" t="inlineStr"/>
+      <c r="AG61" t="inlineStr"/>
+      <c r="AH61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5658,6 +6568,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+      <c r="Y62" t="inlineStr"/>
+      <c r="Z62" t="inlineStr"/>
+      <c r="AA62" t="inlineStr"/>
+      <c r="AB62" t="inlineStr"/>
+      <c r="AC62" t="inlineStr"/>
+      <c r="AD62" t="inlineStr"/>
+      <c r="AE62" t="inlineStr"/>
+      <c r="AF62" t="inlineStr"/>
+      <c r="AG62" t="inlineStr"/>
+      <c r="AH62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5742,6 +6666,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U63" t="inlineStr"/>
+      <c r="V63" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr"/>
+      <c r="Y63" t="inlineStr"/>
+      <c r="Z63" t="inlineStr"/>
+      <c r="AA63" t="inlineStr"/>
+      <c r="AB63" t="inlineStr"/>
+      <c r="AC63" t="inlineStr"/>
+      <c r="AD63" t="inlineStr"/>
+      <c r="AE63" t="inlineStr"/>
+      <c r="AF63" t="inlineStr"/>
+      <c r="AG63" t="inlineStr"/>
+      <c r="AH63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -5826,6 +6764,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+      <c r="Y64" t="inlineStr"/>
+      <c r="Z64" t="inlineStr"/>
+      <c r="AA64" t="inlineStr"/>
+      <c r="AB64" t="inlineStr"/>
+      <c r="AC64" t="inlineStr"/>
+      <c r="AD64" t="inlineStr"/>
+      <c r="AE64" t="inlineStr"/>
+      <c r="AF64" t="inlineStr"/>
+      <c r="AG64" t="inlineStr"/>
+      <c r="AH64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5910,6 +6862,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U65" t="inlineStr"/>
+      <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
+      <c r="Z65" t="inlineStr"/>
+      <c r="AA65" t="inlineStr"/>
+      <c r="AB65" t="inlineStr"/>
+      <c r="AC65" t="inlineStr"/>
+      <c r="AD65" t="inlineStr"/>
+      <c r="AE65" t="inlineStr"/>
+      <c r="AF65" t="inlineStr"/>
+      <c r="AG65" t="inlineStr"/>
+      <c r="AH65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -5994,6 +6960,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U66" t="inlineStr"/>
+      <c r="V66" t="inlineStr"/>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr"/>
+      <c r="Y66" t="inlineStr"/>
+      <c r="Z66" t="inlineStr"/>
+      <c r="AA66" t="inlineStr"/>
+      <c r="AB66" t="inlineStr"/>
+      <c r="AC66" t="inlineStr"/>
+      <c r="AD66" t="inlineStr"/>
+      <c r="AE66" t="inlineStr"/>
+      <c r="AF66" t="inlineStr"/>
+      <c r="AG66" t="inlineStr"/>
+      <c r="AH66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6078,6 +7058,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr"/>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr"/>
+      <c r="Y67" t="inlineStr"/>
+      <c r="Z67" t="inlineStr"/>
+      <c r="AA67" t="inlineStr"/>
+      <c r="AB67" t="inlineStr"/>
+      <c r="AC67" t="inlineStr"/>
+      <c r="AD67" t="inlineStr"/>
+      <c r="AE67" t="inlineStr"/>
+      <c r="AF67" t="inlineStr"/>
+      <c r="AG67" t="inlineStr"/>
+      <c r="AH67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -6162,6 +7156,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr"/>
+      <c r="Y68" t="inlineStr"/>
+      <c r="Z68" t="inlineStr"/>
+      <c r="AA68" t="inlineStr"/>
+      <c r="AB68" t="inlineStr"/>
+      <c r="AC68" t="inlineStr"/>
+      <c r="AD68" t="inlineStr"/>
+      <c r="AE68" t="inlineStr"/>
+      <c r="AF68" t="inlineStr"/>
+      <c r="AG68" t="inlineStr"/>
+      <c r="AH68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6246,6 +7254,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr"/>
+      <c r="Y69" t="inlineStr"/>
+      <c r="Z69" t="inlineStr"/>
+      <c r="AA69" t="inlineStr"/>
+      <c r="AB69" t="inlineStr"/>
+      <c r="AC69" t="inlineStr"/>
+      <c r="AD69" t="inlineStr"/>
+      <c r="AE69" t="inlineStr"/>
+      <c r="AF69" t="inlineStr"/>
+      <c r="AG69" t="inlineStr"/>
+      <c r="AH69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6330,6 +7352,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr"/>
+      <c r="Y70" t="inlineStr"/>
+      <c r="Z70" t="inlineStr"/>
+      <c r="AA70" t="inlineStr"/>
+      <c r="AB70" t="inlineStr"/>
+      <c r="AC70" t="inlineStr"/>
+      <c r="AD70" t="inlineStr"/>
+      <c r="AE70" t="inlineStr"/>
+      <c r="AF70" t="inlineStr"/>
+      <c r="AG70" t="inlineStr"/>
+      <c r="AH70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -6414,6 +7450,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr"/>
+      <c r="Y71" t="inlineStr"/>
+      <c r="Z71" t="inlineStr"/>
+      <c r="AA71" t="inlineStr"/>
+      <c r="AB71" t="inlineStr"/>
+      <c r="AC71" t="inlineStr"/>
+      <c r="AD71" t="inlineStr"/>
+      <c r="AE71" t="inlineStr"/>
+      <c r="AF71" t="inlineStr"/>
+      <c r="AG71" t="inlineStr"/>
+      <c r="AH71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -6498,6 +7548,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U72" t="inlineStr"/>
+      <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr"/>
+      <c r="Y72" t="inlineStr"/>
+      <c r="Z72" t="inlineStr"/>
+      <c r="AA72" t="inlineStr"/>
+      <c r="AB72" t="inlineStr"/>
+      <c r="AC72" t="inlineStr"/>
+      <c r="AD72" t="inlineStr"/>
+      <c r="AE72" t="inlineStr"/>
+      <c r="AF72" t="inlineStr"/>
+      <c r="AG72" t="inlineStr"/>
+      <c r="AH72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -6582,6 +7646,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr"/>
+      <c r="Y73" t="inlineStr"/>
+      <c r="Z73" t="inlineStr"/>
+      <c r="AA73" t="inlineStr"/>
+      <c r="AB73" t="inlineStr"/>
+      <c r="AC73" t="inlineStr"/>
+      <c r="AD73" t="inlineStr"/>
+      <c r="AE73" t="inlineStr"/>
+      <c r="AF73" t="inlineStr"/>
+      <c r="AG73" t="inlineStr"/>
+      <c r="AH73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -6666,6 +7744,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U74" t="inlineStr"/>
+      <c r="V74" t="inlineStr"/>
+      <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr"/>
+      <c r="Y74" t="inlineStr"/>
+      <c r="Z74" t="inlineStr"/>
+      <c r="AA74" t="inlineStr"/>
+      <c r="AB74" t="inlineStr"/>
+      <c r="AC74" t="inlineStr"/>
+      <c r="AD74" t="inlineStr"/>
+      <c r="AE74" t="inlineStr"/>
+      <c r="AF74" t="inlineStr"/>
+      <c r="AG74" t="inlineStr"/>
+      <c r="AH74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -6750,6 +7842,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U75" t="inlineStr"/>
+      <c r="V75" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr"/>
+      <c r="Y75" t="inlineStr"/>
+      <c r="Z75" t="inlineStr"/>
+      <c r="AA75" t="inlineStr"/>
+      <c r="AB75" t="inlineStr"/>
+      <c r="AC75" t="inlineStr"/>
+      <c r="AD75" t="inlineStr"/>
+      <c r="AE75" t="inlineStr"/>
+      <c r="AF75" t="inlineStr"/>
+      <c r="AG75" t="inlineStr"/>
+      <c r="AH75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -6834,6 +7940,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U76" t="inlineStr"/>
+      <c r="V76" t="inlineStr"/>
+      <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr"/>
+      <c r="Y76" t="inlineStr"/>
+      <c r="Z76" t="inlineStr"/>
+      <c r="AA76" t="inlineStr"/>
+      <c r="AB76" t="inlineStr"/>
+      <c r="AC76" t="inlineStr"/>
+      <c r="AD76" t="inlineStr"/>
+      <c r="AE76" t="inlineStr"/>
+      <c r="AF76" t="inlineStr"/>
+      <c r="AG76" t="inlineStr"/>
+      <c r="AH76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -6918,6 +8038,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U77" t="inlineStr"/>
+      <c r="V77" t="inlineStr"/>
+      <c r="W77" t="inlineStr"/>
+      <c r="X77" t="inlineStr"/>
+      <c r="Y77" t="inlineStr"/>
+      <c r="Z77" t="inlineStr"/>
+      <c r="AA77" t="inlineStr"/>
+      <c r="AB77" t="inlineStr"/>
+      <c r="AC77" t="inlineStr"/>
+      <c r="AD77" t="inlineStr"/>
+      <c r="AE77" t="inlineStr"/>
+      <c r="AF77" t="inlineStr"/>
+      <c r="AG77" t="inlineStr"/>
+      <c r="AH77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7002,6 +8136,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U78" t="inlineStr"/>
+      <c r="V78" t="inlineStr"/>
+      <c r="W78" t="inlineStr"/>
+      <c r="X78" t="inlineStr"/>
+      <c r="Y78" t="inlineStr"/>
+      <c r="Z78" t="inlineStr"/>
+      <c r="AA78" t="inlineStr"/>
+      <c r="AB78" t="inlineStr"/>
+      <c r="AC78" t="inlineStr"/>
+      <c r="AD78" t="inlineStr"/>
+      <c r="AE78" t="inlineStr"/>
+      <c r="AF78" t="inlineStr"/>
+      <c r="AG78" t="inlineStr"/>
+      <c r="AH78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7086,6 +8234,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U79" t="inlineStr"/>
+      <c r="V79" t="inlineStr"/>
+      <c r="W79" t="inlineStr"/>
+      <c r="X79" t="inlineStr"/>
+      <c r="Y79" t="inlineStr"/>
+      <c r="Z79" t="inlineStr"/>
+      <c r="AA79" t="inlineStr"/>
+      <c r="AB79" t="inlineStr"/>
+      <c r="AC79" t="inlineStr"/>
+      <c r="AD79" t="inlineStr"/>
+      <c r="AE79" t="inlineStr"/>
+      <c r="AF79" t="inlineStr"/>
+      <c r="AG79" t="inlineStr"/>
+      <c r="AH79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7170,6 +8332,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U80" t="inlineStr"/>
+      <c r="V80" t="inlineStr"/>
+      <c r="W80" t="inlineStr"/>
+      <c r="X80" t="inlineStr"/>
+      <c r="Y80" t="inlineStr"/>
+      <c r="Z80" t="inlineStr"/>
+      <c r="AA80" t="inlineStr"/>
+      <c r="AB80" t="inlineStr"/>
+      <c r="AC80" t="inlineStr"/>
+      <c r="AD80" t="inlineStr"/>
+      <c r="AE80" t="inlineStr"/>
+      <c r="AF80" t="inlineStr"/>
+      <c r="AG80" t="inlineStr"/>
+      <c r="AH80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -7254,6 +8430,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U81" t="inlineStr"/>
+      <c r="V81" t="inlineStr"/>
+      <c r="W81" t="inlineStr"/>
+      <c r="X81" t="inlineStr"/>
+      <c r="Y81" t="inlineStr"/>
+      <c r="Z81" t="inlineStr"/>
+      <c r="AA81" t="inlineStr"/>
+      <c r="AB81" t="inlineStr"/>
+      <c r="AC81" t="inlineStr"/>
+      <c r="AD81" t="inlineStr"/>
+      <c r="AE81" t="inlineStr"/>
+      <c r="AF81" t="inlineStr"/>
+      <c r="AG81" t="inlineStr"/>
+      <c r="AH81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -7338,6 +8528,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U82" t="inlineStr"/>
+      <c r="V82" t="inlineStr"/>
+      <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr"/>
+      <c r="Y82" t="inlineStr"/>
+      <c r="Z82" t="inlineStr"/>
+      <c r="AA82" t="inlineStr"/>
+      <c r="AB82" t="inlineStr"/>
+      <c r="AC82" t="inlineStr"/>
+      <c r="AD82" t="inlineStr"/>
+      <c r="AE82" t="inlineStr"/>
+      <c r="AF82" t="inlineStr"/>
+      <c r="AG82" t="inlineStr"/>
+      <c r="AH82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -7422,6 +8626,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U83" t="inlineStr"/>
+      <c r="V83" t="inlineStr"/>
+      <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr"/>
+      <c r="Y83" t="inlineStr"/>
+      <c r="Z83" t="inlineStr"/>
+      <c r="AA83" t="inlineStr"/>
+      <c r="AB83" t="inlineStr"/>
+      <c r="AC83" t="inlineStr"/>
+      <c r="AD83" t="inlineStr"/>
+      <c r="AE83" t="inlineStr"/>
+      <c r="AF83" t="inlineStr"/>
+      <c r="AG83" t="inlineStr"/>
+      <c r="AH83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -7506,6 +8724,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U84" t="inlineStr"/>
+      <c r="V84" t="inlineStr"/>
+      <c r="W84" t="inlineStr"/>
+      <c r="X84" t="inlineStr"/>
+      <c r="Y84" t="inlineStr"/>
+      <c r="Z84" t="inlineStr"/>
+      <c r="AA84" t="inlineStr"/>
+      <c r="AB84" t="inlineStr"/>
+      <c r="AC84" t="inlineStr"/>
+      <c r="AD84" t="inlineStr"/>
+      <c r="AE84" t="inlineStr"/>
+      <c r="AF84" t="inlineStr"/>
+      <c r="AG84" t="inlineStr"/>
+      <c r="AH84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -7590,6 +8822,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U85" t="inlineStr"/>
+      <c r="V85" t="inlineStr"/>
+      <c r="W85" t="inlineStr"/>
+      <c r="X85" t="inlineStr"/>
+      <c r="Y85" t="inlineStr"/>
+      <c r="Z85" t="inlineStr"/>
+      <c r="AA85" t="inlineStr"/>
+      <c r="AB85" t="inlineStr"/>
+      <c r="AC85" t="inlineStr"/>
+      <c r="AD85" t="inlineStr"/>
+      <c r="AE85" t="inlineStr"/>
+      <c r="AF85" t="inlineStr"/>
+      <c r="AG85" t="inlineStr"/>
+      <c r="AH85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -7674,6 +8920,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U86" t="inlineStr"/>
+      <c r="V86" t="inlineStr"/>
+      <c r="W86" t="inlineStr"/>
+      <c r="X86" t="inlineStr"/>
+      <c r="Y86" t="inlineStr"/>
+      <c r="Z86" t="inlineStr"/>
+      <c r="AA86" t="inlineStr"/>
+      <c r="AB86" t="inlineStr"/>
+      <c r="AC86" t="inlineStr"/>
+      <c r="AD86" t="inlineStr"/>
+      <c r="AE86" t="inlineStr"/>
+      <c r="AF86" t="inlineStr"/>
+      <c r="AG86" t="inlineStr"/>
+      <c r="AH86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -7758,6 +9018,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U87" t="inlineStr"/>
+      <c r="V87" t="inlineStr"/>
+      <c r="W87" t="inlineStr"/>
+      <c r="X87" t="inlineStr"/>
+      <c r="Y87" t="inlineStr"/>
+      <c r="Z87" t="inlineStr"/>
+      <c r="AA87" t="inlineStr"/>
+      <c r="AB87" t="inlineStr"/>
+      <c r="AC87" t="inlineStr"/>
+      <c r="AD87" t="inlineStr"/>
+      <c r="AE87" t="inlineStr"/>
+      <c r="AF87" t="inlineStr"/>
+      <c r="AG87" t="inlineStr"/>
+      <c r="AH87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -7842,6 +9116,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U88" t="inlineStr"/>
+      <c r="V88" t="inlineStr"/>
+      <c r="W88" t="inlineStr"/>
+      <c r="X88" t="inlineStr"/>
+      <c r="Y88" t="inlineStr"/>
+      <c r="Z88" t="inlineStr"/>
+      <c r="AA88" t="inlineStr"/>
+      <c r="AB88" t="inlineStr"/>
+      <c r="AC88" t="inlineStr"/>
+      <c r="AD88" t="inlineStr"/>
+      <c r="AE88" t="inlineStr"/>
+      <c r="AF88" t="inlineStr"/>
+      <c r="AG88" t="inlineStr"/>
+      <c r="AH88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -7926,6 +9214,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U89" t="inlineStr"/>
+      <c r="V89" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
+      <c r="X89" t="inlineStr"/>
+      <c r="Y89" t="inlineStr"/>
+      <c r="Z89" t="inlineStr"/>
+      <c r="AA89" t="inlineStr"/>
+      <c r="AB89" t="inlineStr"/>
+      <c r="AC89" t="inlineStr"/>
+      <c r="AD89" t="inlineStr"/>
+      <c r="AE89" t="inlineStr"/>
+      <c r="AF89" t="inlineStr"/>
+      <c r="AG89" t="inlineStr"/>
+      <c r="AH89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8010,6 +9312,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U90" t="inlineStr"/>
+      <c r="V90" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr"/>
+      <c r="Y90" t="inlineStr"/>
+      <c r="Z90" t="inlineStr"/>
+      <c r="AA90" t="inlineStr"/>
+      <c r="AB90" t="inlineStr"/>
+      <c r="AC90" t="inlineStr"/>
+      <c r="AD90" t="inlineStr"/>
+      <c r="AE90" t="inlineStr"/>
+      <c r="AF90" t="inlineStr"/>
+      <c r="AG90" t="inlineStr"/>
+      <c r="AH90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -8094,6 +9410,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U91" t="inlineStr"/>
+      <c r="V91" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr"/>
+      <c r="Y91" t="inlineStr"/>
+      <c r="Z91" t="inlineStr"/>
+      <c r="AA91" t="inlineStr"/>
+      <c r="AB91" t="inlineStr"/>
+      <c r="AC91" t="inlineStr"/>
+      <c r="AD91" t="inlineStr"/>
+      <c r="AE91" t="inlineStr"/>
+      <c r="AF91" t="inlineStr"/>
+      <c r="AG91" t="inlineStr"/>
+      <c r="AH91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -8178,6 +9508,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U92" t="inlineStr"/>
+      <c r="V92" t="inlineStr"/>
+      <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr"/>
+      <c r="Y92" t="inlineStr"/>
+      <c r="Z92" t="inlineStr"/>
+      <c r="AA92" t="inlineStr"/>
+      <c r="AB92" t="inlineStr"/>
+      <c r="AC92" t="inlineStr"/>
+      <c r="AD92" t="inlineStr"/>
+      <c r="AE92" t="inlineStr"/>
+      <c r="AF92" t="inlineStr"/>
+      <c r="AG92" t="inlineStr"/>
+      <c r="AH92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -8262,6 +9606,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U93" t="inlineStr"/>
+      <c r="V93" t="inlineStr"/>
+      <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr"/>
+      <c r="Y93" t="inlineStr"/>
+      <c r="Z93" t="inlineStr"/>
+      <c r="AA93" t="inlineStr"/>
+      <c r="AB93" t="inlineStr"/>
+      <c r="AC93" t="inlineStr"/>
+      <c r="AD93" t="inlineStr"/>
+      <c r="AE93" t="inlineStr"/>
+      <c r="AF93" t="inlineStr"/>
+      <c r="AG93" t="inlineStr"/>
+      <c r="AH93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -8346,6 +9704,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U94" t="inlineStr"/>
+      <c r="V94" t="inlineStr"/>
+      <c r="W94" t="inlineStr"/>
+      <c r="X94" t="inlineStr"/>
+      <c r="Y94" t="inlineStr"/>
+      <c r="Z94" t="inlineStr"/>
+      <c r="AA94" t="inlineStr"/>
+      <c r="AB94" t="inlineStr"/>
+      <c r="AC94" t="inlineStr"/>
+      <c r="AD94" t="inlineStr"/>
+      <c r="AE94" t="inlineStr"/>
+      <c r="AF94" t="inlineStr"/>
+      <c r="AG94" t="inlineStr"/>
+      <c r="AH94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -8430,6 +9802,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U95" t="inlineStr"/>
+      <c r="V95" t="inlineStr"/>
+      <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr"/>
+      <c r="Y95" t="inlineStr"/>
+      <c r="Z95" t="inlineStr"/>
+      <c r="AA95" t="inlineStr"/>
+      <c r="AB95" t="inlineStr"/>
+      <c r="AC95" t="inlineStr"/>
+      <c r="AD95" t="inlineStr"/>
+      <c r="AE95" t="inlineStr"/>
+      <c r="AF95" t="inlineStr"/>
+      <c r="AG95" t="inlineStr"/>
+      <c r="AH95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -8514,6 +9900,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U96" t="inlineStr"/>
+      <c r="V96" t="inlineStr"/>
+      <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr"/>
+      <c r="Y96" t="inlineStr"/>
+      <c r="Z96" t="inlineStr"/>
+      <c r="AA96" t="inlineStr"/>
+      <c r="AB96" t="inlineStr"/>
+      <c r="AC96" t="inlineStr"/>
+      <c r="AD96" t="inlineStr"/>
+      <c r="AE96" t="inlineStr"/>
+      <c r="AF96" t="inlineStr"/>
+      <c r="AG96" t="inlineStr"/>
+      <c r="AH96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -8598,6 +9998,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U97" t="inlineStr"/>
+      <c r="V97" t="inlineStr"/>
+      <c r="W97" t="inlineStr"/>
+      <c r="X97" t="inlineStr"/>
+      <c r="Y97" t="inlineStr"/>
+      <c r="Z97" t="inlineStr"/>
+      <c r="AA97" t="inlineStr"/>
+      <c r="AB97" t="inlineStr"/>
+      <c r="AC97" t="inlineStr"/>
+      <c r="AD97" t="inlineStr"/>
+      <c r="AE97" t="inlineStr"/>
+      <c r="AF97" t="inlineStr"/>
+      <c r="AG97" t="inlineStr"/>
+      <c r="AH97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -8682,6 +10096,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U98" t="inlineStr"/>
+      <c r="V98" t="inlineStr"/>
+      <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr"/>
+      <c r="Y98" t="inlineStr"/>
+      <c r="Z98" t="inlineStr"/>
+      <c r="AA98" t="inlineStr"/>
+      <c r="AB98" t="inlineStr"/>
+      <c r="AC98" t="inlineStr"/>
+      <c r="AD98" t="inlineStr"/>
+      <c r="AE98" t="inlineStr"/>
+      <c r="AF98" t="inlineStr"/>
+      <c r="AG98" t="inlineStr"/>
+      <c r="AH98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -8766,6 +10194,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr"/>
+      <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr"/>
+      <c r="Y99" t="inlineStr"/>
+      <c r="Z99" t="inlineStr"/>
+      <c r="AA99" t="inlineStr"/>
+      <c r="AB99" t="inlineStr"/>
+      <c r="AC99" t="inlineStr"/>
+      <c r="AD99" t="inlineStr"/>
+      <c r="AE99" t="inlineStr"/>
+      <c r="AF99" t="inlineStr"/>
+      <c r="AG99" t="inlineStr"/>
+      <c r="AH99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -8850,6 +10292,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U100" t="inlineStr"/>
+      <c r="V100" t="inlineStr"/>
+      <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr"/>
+      <c r="Y100" t="inlineStr"/>
+      <c r="Z100" t="inlineStr"/>
+      <c r="AA100" t="inlineStr"/>
+      <c r="AB100" t="inlineStr"/>
+      <c r="AC100" t="inlineStr"/>
+      <c r="AD100" t="inlineStr"/>
+      <c r="AE100" t="inlineStr"/>
+      <c r="AF100" t="inlineStr"/>
+      <c r="AG100" t="inlineStr"/>
+      <c r="AH100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -8934,6 +10390,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U101" t="inlineStr"/>
+      <c r="V101" t="inlineStr"/>
+      <c r="W101" t="inlineStr"/>
+      <c r="X101" t="inlineStr"/>
+      <c r="Y101" t="inlineStr"/>
+      <c r="Z101" t="inlineStr"/>
+      <c r="AA101" t="inlineStr"/>
+      <c r="AB101" t="inlineStr"/>
+      <c r="AC101" t="inlineStr"/>
+      <c r="AD101" t="inlineStr"/>
+      <c r="AE101" t="inlineStr"/>
+      <c r="AF101" t="inlineStr"/>
+      <c r="AG101" t="inlineStr"/>
+      <c r="AH101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -9018,6 +10488,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U102" t="inlineStr"/>
+      <c r="V102" t="inlineStr"/>
+      <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr"/>
+      <c r="Y102" t="inlineStr"/>
+      <c r="Z102" t="inlineStr"/>
+      <c r="AA102" t="inlineStr"/>
+      <c r="AB102" t="inlineStr"/>
+      <c r="AC102" t="inlineStr"/>
+      <c r="AD102" t="inlineStr"/>
+      <c r="AE102" t="inlineStr"/>
+      <c r="AF102" t="inlineStr"/>
+      <c r="AG102" t="inlineStr"/>
+      <c r="AH102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -9102,6 +10586,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U103" t="inlineStr"/>
+      <c r="V103" t="inlineStr"/>
+      <c r="W103" t="inlineStr"/>
+      <c r="X103" t="inlineStr"/>
+      <c r="Y103" t="inlineStr"/>
+      <c r="Z103" t="inlineStr"/>
+      <c r="AA103" t="inlineStr"/>
+      <c r="AB103" t="inlineStr"/>
+      <c r="AC103" t="inlineStr"/>
+      <c r="AD103" t="inlineStr"/>
+      <c r="AE103" t="inlineStr"/>
+      <c r="AF103" t="inlineStr"/>
+      <c r="AG103" t="inlineStr"/>
+      <c r="AH103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -9186,6 +10684,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U104" t="inlineStr"/>
+      <c r="V104" t="inlineStr"/>
+      <c r="W104" t="inlineStr"/>
+      <c r="X104" t="inlineStr"/>
+      <c r="Y104" t="inlineStr"/>
+      <c r="Z104" t="inlineStr"/>
+      <c r="AA104" t="inlineStr"/>
+      <c r="AB104" t="inlineStr"/>
+      <c r="AC104" t="inlineStr"/>
+      <c r="AD104" t="inlineStr"/>
+      <c r="AE104" t="inlineStr"/>
+      <c r="AF104" t="inlineStr"/>
+      <c r="AG104" t="inlineStr"/>
+      <c r="AH104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -9270,6 +10782,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U105" t="inlineStr"/>
+      <c r="V105" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr"/>
+      <c r="Y105" t="inlineStr"/>
+      <c r="Z105" t="inlineStr"/>
+      <c r="AA105" t="inlineStr"/>
+      <c r="AB105" t="inlineStr"/>
+      <c r="AC105" t="inlineStr"/>
+      <c r="AD105" t="inlineStr"/>
+      <c r="AE105" t="inlineStr"/>
+      <c r="AF105" t="inlineStr"/>
+      <c r="AG105" t="inlineStr"/>
+      <c r="AH105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -9354,6 +10880,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U106" t="inlineStr"/>
+      <c r="V106" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
+      <c r="Z106" t="inlineStr"/>
+      <c r="AA106" t="inlineStr"/>
+      <c r="AB106" t="inlineStr"/>
+      <c r="AC106" t="inlineStr"/>
+      <c r="AD106" t="inlineStr"/>
+      <c r="AE106" t="inlineStr"/>
+      <c r="AF106" t="inlineStr"/>
+      <c r="AG106" t="inlineStr"/>
+      <c r="AH106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -9438,6 +10978,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U107" t="inlineStr"/>
+      <c r="V107" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
+      <c r="Z107" t="inlineStr"/>
+      <c r="AA107" t="inlineStr"/>
+      <c r="AB107" t="inlineStr"/>
+      <c r="AC107" t="inlineStr"/>
+      <c r="AD107" t="inlineStr"/>
+      <c r="AE107" t="inlineStr"/>
+      <c r="AF107" t="inlineStr"/>
+      <c r="AG107" t="inlineStr"/>
+      <c r="AH107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -9522,6 +11076,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U108" t="inlineStr"/>
+      <c r="V108" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
+      <c r="X108" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
+      <c r="Z108" t="inlineStr"/>
+      <c r="AA108" t="inlineStr"/>
+      <c r="AB108" t="inlineStr"/>
+      <c r="AC108" t="inlineStr"/>
+      <c r="AD108" t="inlineStr"/>
+      <c r="AE108" t="inlineStr"/>
+      <c r="AF108" t="inlineStr"/>
+      <c r="AG108" t="inlineStr"/>
+      <c r="AH108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -9606,6 +11174,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U109" t="inlineStr"/>
+      <c r="V109" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
+      <c r="Z109" t="inlineStr"/>
+      <c r="AA109" t="inlineStr"/>
+      <c r="AB109" t="inlineStr"/>
+      <c r="AC109" t="inlineStr"/>
+      <c r="AD109" t="inlineStr"/>
+      <c r="AE109" t="inlineStr"/>
+      <c r="AF109" t="inlineStr"/>
+      <c r="AG109" t="inlineStr"/>
+      <c r="AH109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -9690,6 +11272,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U110" t="inlineStr"/>
+      <c r="V110" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
+      <c r="Z110" t="inlineStr"/>
+      <c r="AA110" t="inlineStr"/>
+      <c r="AB110" t="inlineStr"/>
+      <c r="AC110" t="inlineStr"/>
+      <c r="AD110" t="inlineStr"/>
+      <c r="AE110" t="inlineStr"/>
+      <c r="AF110" t="inlineStr"/>
+      <c r="AG110" t="inlineStr"/>
+      <c r="AH110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -9774,6 +11370,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U111" t="inlineStr"/>
+      <c r="V111" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
+      <c r="Z111" t="inlineStr"/>
+      <c r="AA111" t="inlineStr"/>
+      <c r="AB111" t="inlineStr"/>
+      <c r="AC111" t="inlineStr"/>
+      <c r="AD111" t="inlineStr"/>
+      <c r="AE111" t="inlineStr"/>
+      <c r="AF111" t="inlineStr"/>
+      <c r="AG111" t="inlineStr"/>
+      <c r="AH111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -9858,6 +11468,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U112" t="inlineStr"/>
+      <c r="V112" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
+      <c r="Z112" t="inlineStr"/>
+      <c r="AA112" t="inlineStr"/>
+      <c r="AB112" t="inlineStr"/>
+      <c r="AC112" t="inlineStr"/>
+      <c r="AD112" t="inlineStr"/>
+      <c r="AE112" t="inlineStr"/>
+      <c r="AF112" t="inlineStr"/>
+      <c r="AG112" t="inlineStr"/>
+      <c r="AH112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -9942,6 +11566,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U113" t="inlineStr"/>
+      <c r="V113" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
+      <c r="Z113" t="inlineStr"/>
+      <c r="AA113" t="inlineStr"/>
+      <c r="AB113" t="inlineStr"/>
+      <c r="AC113" t="inlineStr"/>
+      <c r="AD113" t="inlineStr"/>
+      <c r="AE113" t="inlineStr"/>
+      <c r="AF113" t="inlineStr"/>
+      <c r="AG113" t="inlineStr"/>
+      <c r="AH113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -10026,6 +11664,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U114" t="inlineStr"/>
+      <c r="V114" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
+      <c r="X114" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
+      <c r="Z114" t="inlineStr"/>
+      <c r="AA114" t="inlineStr"/>
+      <c r="AB114" t="inlineStr"/>
+      <c r="AC114" t="inlineStr"/>
+      <c r="AD114" t="inlineStr"/>
+      <c r="AE114" t="inlineStr"/>
+      <c r="AF114" t="inlineStr"/>
+      <c r="AG114" t="inlineStr"/>
+      <c r="AH114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -10110,6 +11762,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U115" t="inlineStr"/>
+      <c r="V115" t="inlineStr"/>
+      <c r="W115" t="inlineStr"/>
+      <c r="X115" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
+      <c r="Z115" t="inlineStr"/>
+      <c r="AA115" t="inlineStr"/>
+      <c r="AB115" t="inlineStr"/>
+      <c r="AC115" t="inlineStr"/>
+      <c r="AD115" t="inlineStr"/>
+      <c r="AE115" t="inlineStr"/>
+      <c r="AF115" t="inlineStr"/>
+      <c r="AG115" t="inlineStr"/>
+      <c r="AH115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -10194,6 +11860,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U116" t="inlineStr"/>
+      <c r="V116" t="inlineStr"/>
+      <c r="W116" t="inlineStr"/>
+      <c r="X116" t="inlineStr"/>
+      <c r="Y116" t="inlineStr"/>
+      <c r="Z116" t="inlineStr"/>
+      <c r="AA116" t="inlineStr"/>
+      <c r="AB116" t="inlineStr"/>
+      <c r="AC116" t="inlineStr"/>
+      <c r="AD116" t="inlineStr"/>
+      <c r="AE116" t="inlineStr"/>
+      <c r="AF116" t="inlineStr"/>
+      <c r="AG116" t="inlineStr"/>
+      <c r="AH116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -10278,6 +11958,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U117" t="inlineStr"/>
+      <c r="V117" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
+      <c r="X117" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
+      <c r="Z117" t="inlineStr"/>
+      <c r="AA117" t="inlineStr"/>
+      <c r="AB117" t="inlineStr"/>
+      <c r="AC117" t="inlineStr"/>
+      <c r="AD117" t="inlineStr"/>
+      <c r="AE117" t="inlineStr"/>
+      <c r="AF117" t="inlineStr"/>
+      <c r="AG117" t="inlineStr"/>
+      <c r="AH117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -10362,6 +12056,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U118" t="inlineStr"/>
+      <c r="V118" t="inlineStr"/>
+      <c r="W118" t="inlineStr"/>
+      <c r="X118" t="inlineStr"/>
+      <c r="Y118" t="inlineStr"/>
+      <c r="Z118" t="inlineStr"/>
+      <c r="AA118" t="inlineStr"/>
+      <c r="AB118" t="inlineStr"/>
+      <c r="AC118" t="inlineStr"/>
+      <c r="AD118" t="inlineStr"/>
+      <c r="AE118" t="inlineStr"/>
+      <c r="AF118" t="inlineStr"/>
+      <c r="AG118" t="inlineStr"/>
+      <c r="AH118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -10446,6 +12154,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U119" t="inlineStr"/>
+      <c r="V119" t="inlineStr"/>
+      <c r="W119" t="inlineStr"/>
+      <c r="X119" t="inlineStr"/>
+      <c r="Y119" t="inlineStr"/>
+      <c r="Z119" t="inlineStr"/>
+      <c r="AA119" t="inlineStr"/>
+      <c r="AB119" t="inlineStr"/>
+      <c r="AC119" t="inlineStr"/>
+      <c r="AD119" t="inlineStr"/>
+      <c r="AE119" t="inlineStr"/>
+      <c r="AF119" t="inlineStr"/>
+      <c r="AG119" t="inlineStr"/>
+      <c r="AH119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -10530,6 +12252,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U120" t="inlineStr"/>
+      <c r="V120" t="inlineStr"/>
+      <c r="W120" t="inlineStr"/>
+      <c r="X120" t="inlineStr"/>
+      <c r="Y120" t="inlineStr"/>
+      <c r="Z120" t="inlineStr"/>
+      <c r="AA120" t="inlineStr"/>
+      <c r="AB120" t="inlineStr"/>
+      <c r="AC120" t="inlineStr"/>
+      <c r="AD120" t="inlineStr"/>
+      <c r="AE120" t="inlineStr"/>
+      <c r="AF120" t="inlineStr"/>
+      <c r="AG120" t="inlineStr"/>
+      <c r="AH120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -10614,6 +12350,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U121" t="inlineStr"/>
+      <c r="V121" t="inlineStr"/>
+      <c r="W121" t="inlineStr"/>
+      <c r="X121" t="inlineStr"/>
+      <c r="Y121" t="inlineStr"/>
+      <c r="Z121" t="inlineStr"/>
+      <c r="AA121" t="inlineStr"/>
+      <c r="AB121" t="inlineStr"/>
+      <c r="AC121" t="inlineStr"/>
+      <c r="AD121" t="inlineStr"/>
+      <c r="AE121" t="inlineStr"/>
+      <c r="AF121" t="inlineStr"/>
+      <c r="AG121" t="inlineStr"/>
+      <c r="AH121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -10698,6 +12448,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U122" t="inlineStr"/>
+      <c r="V122" t="inlineStr"/>
+      <c r="W122" t="inlineStr"/>
+      <c r="X122" t="inlineStr"/>
+      <c r="Y122" t="inlineStr"/>
+      <c r="Z122" t="inlineStr"/>
+      <c r="AA122" t="inlineStr"/>
+      <c r="AB122" t="inlineStr"/>
+      <c r="AC122" t="inlineStr"/>
+      <c r="AD122" t="inlineStr"/>
+      <c r="AE122" t="inlineStr"/>
+      <c r="AF122" t="inlineStr"/>
+      <c r="AG122" t="inlineStr"/>
+      <c r="AH122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -10782,6 +12546,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U123" t="inlineStr"/>
+      <c r="V123" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
+      <c r="X123" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
+      <c r="Z123" t="inlineStr"/>
+      <c r="AA123" t="inlineStr"/>
+      <c r="AB123" t="inlineStr"/>
+      <c r="AC123" t="inlineStr"/>
+      <c r="AD123" t="inlineStr"/>
+      <c r="AE123" t="inlineStr"/>
+      <c r="AF123" t="inlineStr"/>
+      <c r="AG123" t="inlineStr"/>
+      <c r="AH123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -10866,6 +12644,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U124" t="inlineStr"/>
+      <c r="V124" t="inlineStr"/>
+      <c r="W124" t="inlineStr"/>
+      <c r="X124" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
+      <c r="Z124" t="inlineStr"/>
+      <c r="AA124" t="inlineStr"/>
+      <c r="AB124" t="inlineStr"/>
+      <c r="AC124" t="inlineStr"/>
+      <c r="AD124" t="inlineStr"/>
+      <c r="AE124" t="inlineStr"/>
+      <c r="AF124" t="inlineStr"/>
+      <c r="AG124" t="inlineStr"/>
+      <c r="AH124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -10950,6 +12742,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U125" t="inlineStr"/>
+      <c r="V125" t="inlineStr"/>
+      <c r="W125" t="inlineStr"/>
+      <c r="X125" t="inlineStr"/>
+      <c r="Y125" t="inlineStr"/>
+      <c r="Z125" t="inlineStr"/>
+      <c r="AA125" t="inlineStr"/>
+      <c r="AB125" t="inlineStr"/>
+      <c r="AC125" t="inlineStr"/>
+      <c r="AD125" t="inlineStr"/>
+      <c r="AE125" t="inlineStr"/>
+      <c r="AF125" t="inlineStr"/>
+      <c r="AG125" t="inlineStr"/>
+      <c r="AH125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -11034,6 +12840,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U126" t="inlineStr"/>
+      <c r="V126" t="inlineStr"/>
+      <c r="W126" t="inlineStr"/>
+      <c r="X126" t="inlineStr"/>
+      <c r="Y126" t="inlineStr"/>
+      <c r="Z126" t="inlineStr"/>
+      <c r="AA126" t="inlineStr"/>
+      <c r="AB126" t="inlineStr"/>
+      <c r="AC126" t="inlineStr"/>
+      <c r="AD126" t="inlineStr"/>
+      <c r="AE126" t="inlineStr"/>
+      <c r="AF126" t="inlineStr"/>
+      <c r="AG126" t="inlineStr"/>
+      <c r="AH126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -11118,6 +12938,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U127" t="inlineStr"/>
+      <c r="V127" t="inlineStr"/>
+      <c r="W127" t="inlineStr"/>
+      <c r="X127" t="inlineStr"/>
+      <c r="Y127" t="inlineStr"/>
+      <c r="Z127" t="inlineStr"/>
+      <c r="AA127" t="inlineStr"/>
+      <c r="AB127" t="inlineStr"/>
+      <c r="AC127" t="inlineStr"/>
+      <c r="AD127" t="inlineStr"/>
+      <c r="AE127" t="inlineStr"/>
+      <c r="AF127" t="inlineStr"/>
+      <c r="AG127" t="inlineStr"/>
+      <c r="AH127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -11202,6 +13036,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U128" t="inlineStr"/>
+      <c r="V128" t="inlineStr"/>
+      <c r="W128" t="inlineStr"/>
+      <c r="X128" t="inlineStr"/>
+      <c r="Y128" t="inlineStr"/>
+      <c r="Z128" t="inlineStr"/>
+      <c r="AA128" t="inlineStr"/>
+      <c r="AB128" t="inlineStr"/>
+      <c r="AC128" t="inlineStr"/>
+      <c r="AD128" t="inlineStr"/>
+      <c r="AE128" t="inlineStr"/>
+      <c r="AF128" t="inlineStr"/>
+      <c r="AG128" t="inlineStr"/>
+      <c r="AH128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -11286,6 +13134,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U129" t="inlineStr"/>
+      <c r="V129" t="inlineStr"/>
+      <c r="W129" t="inlineStr"/>
+      <c r="X129" t="inlineStr"/>
+      <c r="Y129" t="inlineStr"/>
+      <c r="Z129" t="inlineStr"/>
+      <c r="AA129" t="inlineStr"/>
+      <c r="AB129" t="inlineStr"/>
+      <c r="AC129" t="inlineStr"/>
+      <c r="AD129" t="inlineStr"/>
+      <c r="AE129" t="inlineStr"/>
+      <c r="AF129" t="inlineStr"/>
+      <c r="AG129" t="inlineStr"/>
+      <c r="AH129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -11370,6 +13232,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U130" t="inlineStr"/>
+      <c r="V130" t="inlineStr"/>
+      <c r="W130" t="inlineStr"/>
+      <c r="X130" t="inlineStr"/>
+      <c r="Y130" t="inlineStr"/>
+      <c r="Z130" t="inlineStr"/>
+      <c r="AA130" t="inlineStr"/>
+      <c r="AB130" t="inlineStr"/>
+      <c r="AC130" t="inlineStr"/>
+      <c r="AD130" t="inlineStr"/>
+      <c r="AE130" t="inlineStr"/>
+      <c r="AF130" t="inlineStr"/>
+      <c r="AG130" t="inlineStr"/>
+      <c r="AH130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -11454,6 +13330,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U131" t="inlineStr"/>
+      <c r="V131" t="inlineStr"/>
+      <c r="W131" t="inlineStr"/>
+      <c r="X131" t="inlineStr"/>
+      <c r="Y131" t="inlineStr"/>
+      <c r="Z131" t="inlineStr"/>
+      <c r="AA131" t="inlineStr"/>
+      <c r="AB131" t="inlineStr"/>
+      <c r="AC131" t="inlineStr"/>
+      <c r="AD131" t="inlineStr"/>
+      <c r="AE131" t="inlineStr"/>
+      <c r="AF131" t="inlineStr"/>
+      <c r="AG131" t="inlineStr"/>
+      <c r="AH131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -11538,6 +13428,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U132" t="inlineStr"/>
+      <c r="V132" t="inlineStr"/>
+      <c r="W132" t="inlineStr"/>
+      <c r="X132" t="inlineStr"/>
+      <c r="Y132" t="inlineStr"/>
+      <c r="Z132" t="inlineStr"/>
+      <c r="AA132" t="inlineStr"/>
+      <c r="AB132" t="inlineStr"/>
+      <c r="AC132" t="inlineStr"/>
+      <c r="AD132" t="inlineStr"/>
+      <c r="AE132" t="inlineStr"/>
+      <c r="AF132" t="inlineStr"/>
+      <c r="AG132" t="inlineStr"/>
+      <c r="AH132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -11622,6 +13526,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U133" t="inlineStr"/>
+      <c r="V133" t="inlineStr"/>
+      <c r="W133" t="inlineStr"/>
+      <c r="X133" t="inlineStr"/>
+      <c r="Y133" t="inlineStr"/>
+      <c r="Z133" t="inlineStr"/>
+      <c r="AA133" t="inlineStr"/>
+      <c r="AB133" t="inlineStr"/>
+      <c r="AC133" t="inlineStr"/>
+      <c r="AD133" t="inlineStr"/>
+      <c r="AE133" t="inlineStr"/>
+      <c r="AF133" t="inlineStr"/>
+      <c r="AG133" t="inlineStr"/>
+      <c r="AH133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -11706,6 +13624,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U134" t="inlineStr"/>
+      <c r="V134" t="inlineStr"/>
+      <c r="W134" t="inlineStr"/>
+      <c r="X134" t="inlineStr"/>
+      <c r="Y134" t="inlineStr"/>
+      <c r="Z134" t="inlineStr"/>
+      <c r="AA134" t="inlineStr"/>
+      <c r="AB134" t="inlineStr"/>
+      <c r="AC134" t="inlineStr"/>
+      <c r="AD134" t="inlineStr"/>
+      <c r="AE134" t="inlineStr"/>
+      <c r="AF134" t="inlineStr"/>
+      <c r="AG134" t="inlineStr"/>
+      <c r="AH134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -11790,6 +13722,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U135" t="inlineStr"/>
+      <c r="V135" t="inlineStr"/>
+      <c r="W135" t="inlineStr"/>
+      <c r="X135" t="inlineStr"/>
+      <c r="Y135" t="inlineStr"/>
+      <c r="Z135" t="inlineStr"/>
+      <c r="AA135" t="inlineStr"/>
+      <c r="AB135" t="inlineStr"/>
+      <c r="AC135" t="inlineStr"/>
+      <c r="AD135" t="inlineStr"/>
+      <c r="AE135" t="inlineStr"/>
+      <c r="AF135" t="inlineStr"/>
+      <c r="AG135" t="inlineStr"/>
+      <c r="AH135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -11874,6 +13820,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U136" t="inlineStr"/>
+      <c r="V136" t="inlineStr"/>
+      <c r="W136" t="inlineStr"/>
+      <c r="X136" t="inlineStr"/>
+      <c r="Y136" t="inlineStr"/>
+      <c r="Z136" t="inlineStr"/>
+      <c r="AA136" t="inlineStr"/>
+      <c r="AB136" t="inlineStr"/>
+      <c r="AC136" t="inlineStr"/>
+      <c r="AD136" t="inlineStr"/>
+      <c r="AE136" t="inlineStr"/>
+      <c r="AF136" t="inlineStr"/>
+      <c r="AG136" t="inlineStr"/>
+      <c r="AH136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -11958,6 +13918,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U137" t="inlineStr"/>
+      <c r="V137" t="inlineStr"/>
+      <c r="W137" t="inlineStr"/>
+      <c r="X137" t="inlineStr"/>
+      <c r="Y137" t="inlineStr"/>
+      <c r="Z137" t="inlineStr"/>
+      <c r="AA137" t="inlineStr"/>
+      <c r="AB137" t="inlineStr"/>
+      <c r="AC137" t="inlineStr"/>
+      <c r="AD137" t="inlineStr"/>
+      <c r="AE137" t="inlineStr"/>
+      <c r="AF137" t="inlineStr"/>
+      <c r="AG137" t="inlineStr"/>
+      <c r="AH137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -12042,6 +14016,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U138" t="inlineStr"/>
+      <c r="V138" t="inlineStr"/>
+      <c r="W138" t="inlineStr"/>
+      <c r="X138" t="inlineStr"/>
+      <c r="Y138" t="inlineStr"/>
+      <c r="Z138" t="inlineStr"/>
+      <c r="AA138" t="inlineStr"/>
+      <c r="AB138" t="inlineStr"/>
+      <c r="AC138" t="inlineStr"/>
+      <c r="AD138" t="inlineStr"/>
+      <c r="AE138" t="inlineStr"/>
+      <c r="AF138" t="inlineStr"/>
+      <c r="AG138" t="inlineStr"/>
+      <c r="AH138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -12126,6 +14114,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U139" t="inlineStr"/>
+      <c r="V139" t="inlineStr"/>
+      <c r="W139" t="inlineStr"/>
+      <c r="X139" t="inlineStr"/>
+      <c r="Y139" t="inlineStr"/>
+      <c r="Z139" t="inlineStr"/>
+      <c r="AA139" t="inlineStr"/>
+      <c r="AB139" t="inlineStr"/>
+      <c r="AC139" t="inlineStr"/>
+      <c r="AD139" t="inlineStr"/>
+      <c r="AE139" t="inlineStr"/>
+      <c r="AF139" t="inlineStr"/>
+      <c r="AG139" t="inlineStr"/>
+      <c r="AH139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -12210,6 +14212,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U140" t="inlineStr"/>
+      <c r="V140" t="inlineStr"/>
+      <c r="W140" t="inlineStr"/>
+      <c r="X140" t="inlineStr"/>
+      <c r="Y140" t="inlineStr"/>
+      <c r="Z140" t="inlineStr"/>
+      <c r="AA140" t="inlineStr"/>
+      <c r="AB140" t="inlineStr"/>
+      <c r="AC140" t="inlineStr"/>
+      <c r="AD140" t="inlineStr"/>
+      <c r="AE140" t="inlineStr"/>
+      <c r="AF140" t="inlineStr"/>
+      <c r="AG140" t="inlineStr"/>
+      <c r="AH140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -12294,6 +14310,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U141" t="inlineStr"/>
+      <c r="V141" t="inlineStr"/>
+      <c r="W141" t="inlineStr"/>
+      <c r="X141" t="inlineStr"/>
+      <c r="Y141" t="inlineStr"/>
+      <c r="Z141" t="inlineStr"/>
+      <c r="AA141" t="inlineStr"/>
+      <c r="AB141" t="inlineStr"/>
+      <c r="AC141" t="inlineStr"/>
+      <c r="AD141" t="inlineStr"/>
+      <c r="AE141" t="inlineStr"/>
+      <c r="AF141" t="inlineStr"/>
+      <c r="AG141" t="inlineStr"/>
+      <c r="AH141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -12378,6 +14408,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U142" t="inlineStr"/>
+      <c r="V142" t="inlineStr"/>
+      <c r="W142" t="inlineStr"/>
+      <c r="X142" t="inlineStr"/>
+      <c r="Y142" t="inlineStr"/>
+      <c r="Z142" t="inlineStr"/>
+      <c r="AA142" t="inlineStr"/>
+      <c r="AB142" t="inlineStr"/>
+      <c r="AC142" t="inlineStr"/>
+      <c r="AD142" t="inlineStr"/>
+      <c r="AE142" t="inlineStr"/>
+      <c r="AF142" t="inlineStr"/>
+      <c r="AG142" t="inlineStr"/>
+      <c r="AH142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -12462,6 +14506,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U143" t="inlineStr"/>
+      <c r="V143" t="inlineStr"/>
+      <c r="W143" t="inlineStr"/>
+      <c r="X143" t="inlineStr"/>
+      <c r="Y143" t="inlineStr"/>
+      <c r="Z143" t="inlineStr"/>
+      <c r="AA143" t="inlineStr"/>
+      <c r="AB143" t="inlineStr"/>
+      <c r="AC143" t="inlineStr"/>
+      <c r="AD143" t="inlineStr"/>
+      <c r="AE143" t="inlineStr"/>
+      <c r="AF143" t="inlineStr"/>
+      <c r="AG143" t="inlineStr"/>
+      <c r="AH143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -12546,6 +14604,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U144" t="inlineStr"/>
+      <c r="V144" t="inlineStr"/>
+      <c r="W144" t="inlineStr"/>
+      <c r="X144" t="inlineStr"/>
+      <c r="Y144" t="inlineStr"/>
+      <c r="Z144" t="inlineStr"/>
+      <c r="AA144" t="inlineStr"/>
+      <c r="AB144" t="inlineStr"/>
+      <c r="AC144" t="inlineStr"/>
+      <c r="AD144" t="inlineStr"/>
+      <c r="AE144" t="inlineStr"/>
+      <c r="AF144" t="inlineStr"/>
+      <c r="AG144" t="inlineStr"/>
+      <c r="AH144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -12630,6 +14702,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U145" t="inlineStr"/>
+      <c r="V145" t="inlineStr"/>
+      <c r="W145" t="inlineStr"/>
+      <c r="X145" t="inlineStr"/>
+      <c r="Y145" t="inlineStr"/>
+      <c r="Z145" t="inlineStr"/>
+      <c r="AA145" t="inlineStr"/>
+      <c r="AB145" t="inlineStr"/>
+      <c r="AC145" t="inlineStr"/>
+      <c r="AD145" t="inlineStr"/>
+      <c r="AE145" t="inlineStr"/>
+      <c r="AF145" t="inlineStr"/>
+      <c r="AG145" t="inlineStr"/>
+      <c r="AH145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -12714,6 +14800,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U146" t="inlineStr"/>
+      <c r="V146" t="inlineStr"/>
+      <c r="W146" t="inlineStr"/>
+      <c r="X146" t="inlineStr"/>
+      <c r="Y146" t="inlineStr"/>
+      <c r="Z146" t="inlineStr"/>
+      <c r="AA146" t="inlineStr"/>
+      <c r="AB146" t="inlineStr"/>
+      <c r="AC146" t="inlineStr"/>
+      <c r="AD146" t="inlineStr"/>
+      <c r="AE146" t="inlineStr"/>
+      <c r="AF146" t="inlineStr"/>
+      <c r="AG146" t="inlineStr"/>
+      <c r="AH146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -12798,6 +14898,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U147" t="inlineStr"/>
+      <c r="V147" t="inlineStr"/>
+      <c r="W147" t="inlineStr"/>
+      <c r="X147" t="inlineStr"/>
+      <c r="Y147" t="inlineStr"/>
+      <c r="Z147" t="inlineStr"/>
+      <c r="AA147" t="inlineStr"/>
+      <c r="AB147" t="inlineStr"/>
+      <c r="AC147" t="inlineStr"/>
+      <c r="AD147" t="inlineStr"/>
+      <c r="AE147" t="inlineStr"/>
+      <c r="AF147" t="inlineStr"/>
+      <c r="AG147" t="inlineStr"/>
+      <c r="AH147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -12882,6 +14996,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U148" t="inlineStr"/>
+      <c r="V148" t="inlineStr"/>
+      <c r="W148" t="inlineStr"/>
+      <c r="X148" t="inlineStr"/>
+      <c r="Y148" t="inlineStr"/>
+      <c r="Z148" t="inlineStr"/>
+      <c r="AA148" t="inlineStr"/>
+      <c r="AB148" t="inlineStr"/>
+      <c r="AC148" t="inlineStr"/>
+      <c r="AD148" t="inlineStr"/>
+      <c r="AE148" t="inlineStr"/>
+      <c r="AF148" t="inlineStr"/>
+      <c r="AG148" t="inlineStr"/>
+      <c r="AH148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -12966,6 +15094,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U149" t="inlineStr"/>
+      <c r="V149" t="inlineStr"/>
+      <c r="W149" t="inlineStr"/>
+      <c r="X149" t="inlineStr"/>
+      <c r="Y149" t="inlineStr"/>
+      <c r="Z149" t="inlineStr"/>
+      <c r="AA149" t="inlineStr"/>
+      <c r="AB149" t="inlineStr"/>
+      <c r="AC149" t="inlineStr"/>
+      <c r="AD149" t="inlineStr"/>
+      <c r="AE149" t="inlineStr"/>
+      <c r="AF149" t="inlineStr"/>
+      <c r="AG149" t="inlineStr"/>
+      <c r="AH149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -13050,6 +15192,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U150" t="inlineStr"/>
+      <c r="V150" t="inlineStr"/>
+      <c r="W150" t="inlineStr"/>
+      <c r="X150" t="inlineStr"/>
+      <c r="Y150" t="inlineStr"/>
+      <c r="Z150" t="inlineStr"/>
+      <c r="AA150" t="inlineStr"/>
+      <c r="AB150" t="inlineStr"/>
+      <c r="AC150" t="inlineStr"/>
+      <c r="AD150" t="inlineStr"/>
+      <c r="AE150" t="inlineStr"/>
+      <c r="AF150" t="inlineStr"/>
+      <c r="AG150" t="inlineStr"/>
+      <c r="AH150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -13134,6 +15290,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U151" t="inlineStr"/>
+      <c r="V151" t="inlineStr"/>
+      <c r="W151" t="inlineStr"/>
+      <c r="X151" t="inlineStr"/>
+      <c r="Y151" t="inlineStr"/>
+      <c r="Z151" t="inlineStr"/>
+      <c r="AA151" t="inlineStr"/>
+      <c r="AB151" t="inlineStr"/>
+      <c r="AC151" t="inlineStr"/>
+      <c r="AD151" t="inlineStr"/>
+      <c r="AE151" t="inlineStr"/>
+      <c r="AF151" t="inlineStr"/>
+      <c r="AG151" t="inlineStr"/>
+      <c r="AH151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -13218,6 +15388,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U152" t="inlineStr"/>
+      <c r="V152" t="inlineStr"/>
+      <c r="W152" t="inlineStr"/>
+      <c r="X152" t="inlineStr"/>
+      <c r="Y152" t="inlineStr"/>
+      <c r="Z152" t="inlineStr"/>
+      <c r="AA152" t="inlineStr"/>
+      <c r="AB152" t="inlineStr"/>
+      <c r="AC152" t="inlineStr"/>
+      <c r="AD152" t="inlineStr"/>
+      <c r="AE152" t="inlineStr"/>
+      <c r="AF152" t="inlineStr"/>
+      <c r="AG152" t="inlineStr"/>
+      <c r="AH152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -13302,6 +15486,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" t="inlineStr"/>
+      <c r="W153" t="inlineStr"/>
+      <c r="X153" t="inlineStr"/>
+      <c r="Y153" t="inlineStr"/>
+      <c r="Z153" t="inlineStr"/>
+      <c r="AA153" t="inlineStr"/>
+      <c r="AB153" t="inlineStr"/>
+      <c r="AC153" t="inlineStr"/>
+      <c r="AD153" t="inlineStr"/>
+      <c r="AE153" t="inlineStr"/>
+      <c r="AF153" t="inlineStr"/>
+      <c r="AG153" t="inlineStr"/>
+      <c r="AH153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -13386,6 +15584,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U154" t="inlineStr"/>
+      <c r="V154" t="inlineStr"/>
+      <c r="W154" t="inlineStr"/>
+      <c r="X154" t="inlineStr"/>
+      <c r="Y154" t="inlineStr"/>
+      <c r="Z154" t="inlineStr"/>
+      <c r="AA154" t="inlineStr"/>
+      <c r="AB154" t="inlineStr"/>
+      <c r="AC154" t="inlineStr"/>
+      <c r="AD154" t="inlineStr"/>
+      <c r="AE154" t="inlineStr"/>
+      <c r="AF154" t="inlineStr"/>
+      <c r="AG154" t="inlineStr"/>
+      <c r="AH154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -13470,6 +15682,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U155" t="inlineStr"/>
+      <c r="V155" t="inlineStr"/>
+      <c r="W155" t="inlineStr"/>
+      <c r="X155" t="inlineStr"/>
+      <c r="Y155" t="inlineStr"/>
+      <c r="Z155" t="inlineStr"/>
+      <c r="AA155" t="inlineStr"/>
+      <c r="AB155" t="inlineStr"/>
+      <c r="AC155" t="inlineStr"/>
+      <c r="AD155" t="inlineStr"/>
+      <c r="AE155" t="inlineStr"/>
+      <c r="AF155" t="inlineStr"/>
+      <c r="AG155" t="inlineStr"/>
+      <c r="AH155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -13554,6 +15780,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U156" t="inlineStr"/>
+      <c r="V156" t="inlineStr"/>
+      <c r="W156" t="inlineStr"/>
+      <c r="X156" t="inlineStr"/>
+      <c r="Y156" t="inlineStr"/>
+      <c r="Z156" t="inlineStr"/>
+      <c r="AA156" t="inlineStr"/>
+      <c r="AB156" t="inlineStr"/>
+      <c r="AC156" t="inlineStr"/>
+      <c r="AD156" t="inlineStr"/>
+      <c r="AE156" t="inlineStr"/>
+      <c r="AF156" t="inlineStr"/>
+      <c r="AG156" t="inlineStr"/>
+      <c r="AH156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -13638,6 +15878,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U157" t="inlineStr"/>
+      <c r="V157" t="inlineStr"/>
+      <c r="W157" t="inlineStr"/>
+      <c r="X157" t="inlineStr"/>
+      <c r="Y157" t="inlineStr"/>
+      <c r="Z157" t="inlineStr"/>
+      <c r="AA157" t="inlineStr"/>
+      <c r="AB157" t="inlineStr"/>
+      <c r="AC157" t="inlineStr"/>
+      <c r="AD157" t="inlineStr"/>
+      <c r="AE157" t="inlineStr"/>
+      <c r="AF157" t="inlineStr"/>
+      <c r="AG157" t="inlineStr"/>
+      <c r="AH157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -13722,6 +15976,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U158" t="inlineStr"/>
+      <c r="V158" t="inlineStr"/>
+      <c r="W158" t="inlineStr"/>
+      <c r="X158" t="inlineStr"/>
+      <c r="Y158" t="inlineStr"/>
+      <c r="Z158" t="inlineStr"/>
+      <c r="AA158" t="inlineStr"/>
+      <c r="AB158" t="inlineStr"/>
+      <c r="AC158" t="inlineStr"/>
+      <c r="AD158" t="inlineStr"/>
+      <c r="AE158" t="inlineStr"/>
+      <c r="AF158" t="inlineStr"/>
+      <c r="AG158" t="inlineStr"/>
+      <c r="AH158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -13806,6 +16074,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U159" t="inlineStr"/>
+      <c r="V159" t="inlineStr"/>
+      <c r="W159" t="inlineStr"/>
+      <c r="X159" t="inlineStr"/>
+      <c r="Y159" t="inlineStr"/>
+      <c r="Z159" t="inlineStr"/>
+      <c r="AA159" t="inlineStr"/>
+      <c r="AB159" t="inlineStr"/>
+      <c r="AC159" t="inlineStr"/>
+      <c r="AD159" t="inlineStr"/>
+      <c r="AE159" t="inlineStr"/>
+      <c r="AF159" t="inlineStr"/>
+      <c r="AG159" t="inlineStr"/>
+      <c r="AH159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -13890,6 +16172,20 @@
           <t>ممتاز! استمر على هذا الأداء</t>
         </is>
       </c>
+      <c r="U160" t="inlineStr"/>
+      <c r="V160" t="inlineStr"/>
+      <c r="W160" t="inlineStr"/>
+      <c r="X160" t="inlineStr"/>
+      <c r="Y160" t="inlineStr"/>
+      <c r="Z160" t="inlineStr"/>
+      <c r="AA160" t="inlineStr"/>
+      <c r="AB160" t="inlineStr"/>
+      <c r="AC160" t="inlineStr"/>
+      <c r="AD160" t="inlineStr"/>
+      <c r="AE160" t="inlineStr"/>
+      <c r="AF160" t="inlineStr"/>
+      <c r="AG160" t="inlineStr"/>
+      <c r="AH160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -13974,6 +16270,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U161" t="inlineStr"/>
+      <c r="V161" t="inlineStr"/>
+      <c r="W161" t="inlineStr"/>
+      <c r="X161" t="inlineStr"/>
+      <c r="Y161" t="inlineStr"/>
+      <c r="Z161" t="inlineStr"/>
+      <c r="AA161" t="inlineStr"/>
+      <c r="AB161" t="inlineStr"/>
+      <c r="AC161" t="inlineStr"/>
+      <c r="AD161" t="inlineStr"/>
+      <c r="AE161" t="inlineStr"/>
+      <c r="AF161" t="inlineStr"/>
+      <c r="AG161" t="inlineStr"/>
+      <c r="AH161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -14058,6 +16368,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U162" t="inlineStr"/>
+      <c r="V162" t="inlineStr"/>
+      <c r="W162" t="inlineStr"/>
+      <c r="X162" t="inlineStr"/>
+      <c r="Y162" t="inlineStr"/>
+      <c r="Z162" t="inlineStr"/>
+      <c r="AA162" t="inlineStr"/>
+      <c r="AB162" t="inlineStr"/>
+      <c r="AC162" t="inlineStr"/>
+      <c r="AD162" t="inlineStr"/>
+      <c r="AE162" t="inlineStr"/>
+      <c r="AF162" t="inlineStr"/>
+      <c r="AG162" t="inlineStr"/>
+      <c r="AH162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -14142,6 +16466,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U163" t="inlineStr"/>
+      <c r="V163" t="inlineStr"/>
+      <c r="W163" t="inlineStr"/>
+      <c r="X163" t="inlineStr"/>
+      <c r="Y163" t="inlineStr"/>
+      <c r="Z163" t="inlineStr"/>
+      <c r="AA163" t="inlineStr"/>
+      <c r="AB163" t="inlineStr"/>
+      <c r="AC163" t="inlineStr"/>
+      <c r="AD163" t="inlineStr"/>
+      <c r="AE163" t="inlineStr"/>
+      <c r="AF163" t="inlineStr"/>
+      <c r="AG163" t="inlineStr"/>
+      <c r="AH163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -14226,6 +16564,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U164" t="inlineStr"/>
+      <c r="V164" t="inlineStr"/>
+      <c r="W164" t="inlineStr"/>
+      <c r="X164" t="inlineStr"/>
+      <c r="Y164" t="inlineStr"/>
+      <c r="Z164" t="inlineStr"/>
+      <c r="AA164" t="inlineStr"/>
+      <c r="AB164" t="inlineStr"/>
+      <c r="AC164" t="inlineStr"/>
+      <c r="AD164" t="inlineStr"/>
+      <c r="AE164" t="inlineStr"/>
+      <c r="AF164" t="inlineStr"/>
+      <c r="AG164" t="inlineStr"/>
+      <c r="AH164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -14310,6 +16662,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U165" t="inlineStr"/>
+      <c r="V165" t="inlineStr"/>
+      <c r="W165" t="inlineStr"/>
+      <c r="X165" t="inlineStr"/>
+      <c r="Y165" t="inlineStr"/>
+      <c r="Z165" t="inlineStr"/>
+      <c r="AA165" t="inlineStr"/>
+      <c r="AB165" t="inlineStr"/>
+      <c r="AC165" t="inlineStr"/>
+      <c r="AD165" t="inlineStr"/>
+      <c r="AE165" t="inlineStr"/>
+      <c r="AF165" t="inlineStr"/>
+      <c r="AG165" t="inlineStr"/>
+      <c r="AH165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -14394,6 +16760,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U166" t="inlineStr"/>
+      <c r="V166" t="inlineStr"/>
+      <c r="W166" t="inlineStr"/>
+      <c r="X166" t="inlineStr"/>
+      <c r="Y166" t="inlineStr"/>
+      <c r="Z166" t="inlineStr"/>
+      <c r="AA166" t="inlineStr"/>
+      <c r="AB166" t="inlineStr"/>
+      <c r="AC166" t="inlineStr"/>
+      <c r="AD166" t="inlineStr"/>
+      <c r="AE166" t="inlineStr"/>
+      <c r="AF166" t="inlineStr"/>
+      <c r="AG166" t="inlineStr"/>
+      <c r="AH166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -14478,6 +16858,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U167" t="inlineStr"/>
+      <c r="V167" t="inlineStr"/>
+      <c r="W167" t="inlineStr"/>
+      <c r="X167" t="inlineStr"/>
+      <c r="Y167" t="inlineStr"/>
+      <c r="Z167" t="inlineStr"/>
+      <c r="AA167" t="inlineStr"/>
+      <c r="AB167" t="inlineStr"/>
+      <c r="AC167" t="inlineStr"/>
+      <c r="AD167" t="inlineStr"/>
+      <c r="AE167" t="inlineStr"/>
+      <c r="AF167" t="inlineStr"/>
+      <c r="AG167" t="inlineStr"/>
+      <c r="AH167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -14562,6 +16956,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U168" t="inlineStr"/>
+      <c r="V168" t="inlineStr"/>
+      <c r="W168" t="inlineStr"/>
+      <c r="X168" t="inlineStr"/>
+      <c r="Y168" t="inlineStr"/>
+      <c r="Z168" t="inlineStr"/>
+      <c r="AA168" t="inlineStr"/>
+      <c r="AB168" t="inlineStr"/>
+      <c r="AC168" t="inlineStr"/>
+      <c r="AD168" t="inlineStr"/>
+      <c r="AE168" t="inlineStr"/>
+      <c r="AF168" t="inlineStr"/>
+      <c r="AG168" t="inlineStr"/>
+      <c r="AH168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -14646,6 +17054,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U169" t="inlineStr"/>
+      <c r="V169" t="inlineStr"/>
+      <c r="W169" t="inlineStr"/>
+      <c r="X169" t="inlineStr"/>
+      <c r="Y169" t="inlineStr"/>
+      <c r="Z169" t="inlineStr"/>
+      <c r="AA169" t="inlineStr"/>
+      <c r="AB169" t="inlineStr"/>
+      <c r="AC169" t="inlineStr"/>
+      <c r="AD169" t="inlineStr"/>
+      <c r="AE169" t="inlineStr"/>
+      <c r="AF169" t="inlineStr"/>
+      <c r="AG169" t="inlineStr"/>
+      <c r="AH169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -14730,6 +17152,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U170" t="inlineStr"/>
+      <c r="V170" t="inlineStr"/>
+      <c r="W170" t="inlineStr"/>
+      <c r="X170" t="inlineStr"/>
+      <c r="Y170" t="inlineStr"/>
+      <c r="Z170" t="inlineStr"/>
+      <c r="AA170" t="inlineStr"/>
+      <c r="AB170" t="inlineStr"/>
+      <c r="AC170" t="inlineStr"/>
+      <c r="AD170" t="inlineStr"/>
+      <c r="AE170" t="inlineStr"/>
+      <c r="AF170" t="inlineStr"/>
+      <c r="AG170" t="inlineStr"/>
+      <c r="AH170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -14814,6 +17250,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U171" t="inlineStr"/>
+      <c r="V171" t="inlineStr"/>
+      <c r="W171" t="inlineStr"/>
+      <c r="X171" t="inlineStr"/>
+      <c r="Y171" t="inlineStr"/>
+      <c r="Z171" t="inlineStr"/>
+      <c r="AA171" t="inlineStr"/>
+      <c r="AB171" t="inlineStr"/>
+      <c r="AC171" t="inlineStr"/>
+      <c r="AD171" t="inlineStr"/>
+      <c r="AE171" t="inlineStr"/>
+      <c r="AF171" t="inlineStr"/>
+      <c r="AG171" t="inlineStr"/>
+      <c r="AH171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -14898,6 +17348,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U172" t="inlineStr"/>
+      <c r="V172" t="inlineStr"/>
+      <c r="W172" t="inlineStr"/>
+      <c r="X172" t="inlineStr"/>
+      <c r="Y172" t="inlineStr"/>
+      <c r="Z172" t="inlineStr"/>
+      <c r="AA172" t="inlineStr"/>
+      <c r="AB172" t="inlineStr"/>
+      <c r="AC172" t="inlineStr"/>
+      <c r="AD172" t="inlineStr"/>
+      <c r="AE172" t="inlineStr"/>
+      <c r="AF172" t="inlineStr"/>
+      <c r="AG172" t="inlineStr"/>
+      <c r="AH172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -14982,6 +17446,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U173" t="inlineStr"/>
+      <c r="V173" t="inlineStr"/>
+      <c r="W173" t="inlineStr"/>
+      <c r="X173" t="inlineStr"/>
+      <c r="Y173" t="inlineStr"/>
+      <c r="Z173" t="inlineStr"/>
+      <c r="AA173" t="inlineStr"/>
+      <c r="AB173" t="inlineStr"/>
+      <c r="AC173" t="inlineStr"/>
+      <c r="AD173" t="inlineStr"/>
+      <c r="AE173" t="inlineStr"/>
+      <c r="AF173" t="inlineStr"/>
+      <c r="AG173" t="inlineStr"/>
+      <c r="AH173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -15066,6 +17544,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U174" t="inlineStr"/>
+      <c r="V174" t="inlineStr"/>
+      <c r="W174" t="inlineStr"/>
+      <c r="X174" t="inlineStr"/>
+      <c r="Y174" t="inlineStr"/>
+      <c r="Z174" t="inlineStr"/>
+      <c r="AA174" t="inlineStr"/>
+      <c r="AB174" t="inlineStr"/>
+      <c r="AC174" t="inlineStr"/>
+      <c r="AD174" t="inlineStr"/>
+      <c r="AE174" t="inlineStr"/>
+      <c r="AF174" t="inlineStr"/>
+      <c r="AG174" t="inlineStr"/>
+      <c r="AH174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -15150,6 +17642,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U175" t="inlineStr"/>
+      <c r="V175" t="inlineStr"/>
+      <c r="W175" t="inlineStr"/>
+      <c r="X175" t="inlineStr"/>
+      <c r="Y175" t="inlineStr"/>
+      <c r="Z175" t="inlineStr"/>
+      <c r="AA175" t="inlineStr"/>
+      <c r="AB175" t="inlineStr"/>
+      <c r="AC175" t="inlineStr"/>
+      <c r="AD175" t="inlineStr"/>
+      <c r="AE175" t="inlineStr"/>
+      <c r="AF175" t="inlineStr"/>
+      <c r="AG175" t="inlineStr"/>
+      <c r="AH175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -15234,6 +17740,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U176" t="inlineStr"/>
+      <c r="V176" t="inlineStr"/>
+      <c r="W176" t="inlineStr"/>
+      <c r="X176" t="inlineStr"/>
+      <c r="Y176" t="inlineStr"/>
+      <c r="Z176" t="inlineStr"/>
+      <c r="AA176" t="inlineStr"/>
+      <c r="AB176" t="inlineStr"/>
+      <c r="AC176" t="inlineStr"/>
+      <c r="AD176" t="inlineStr"/>
+      <c r="AE176" t="inlineStr"/>
+      <c r="AF176" t="inlineStr"/>
+      <c r="AG176" t="inlineStr"/>
+      <c r="AH176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -15318,6 +17838,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U177" t="inlineStr"/>
+      <c r="V177" t="inlineStr"/>
+      <c r="W177" t="inlineStr"/>
+      <c r="X177" t="inlineStr"/>
+      <c r="Y177" t="inlineStr"/>
+      <c r="Z177" t="inlineStr"/>
+      <c r="AA177" t="inlineStr"/>
+      <c r="AB177" t="inlineStr"/>
+      <c r="AC177" t="inlineStr"/>
+      <c r="AD177" t="inlineStr"/>
+      <c r="AE177" t="inlineStr"/>
+      <c r="AF177" t="inlineStr"/>
+      <c r="AG177" t="inlineStr"/>
+      <c r="AH177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -15402,6 +17936,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U178" t="inlineStr"/>
+      <c r="V178" t="inlineStr"/>
+      <c r="W178" t="inlineStr"/>
+      <c r="X178" t="inlineStr"/>
+      <c r="Y178" t="inlineStr"/>
+      <c r="Z178" t="inlineStr"/>
+      <c r="AA178" t="inlineStr"/>
+      <c r="AB178" t="inlineStr"/>
+      <c r="AC178" t="inlineStr"/>
+      <c r="AD178" t="inlineStr"/>
+      <c r="AE178" t="inlineStr"/>
+      <c r="AF178" t="inlineStr"/>
+      <c r="AG178" t="inlineStr"/>
+      <c r="AH178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -15486,6 +18034,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U179" t="inlineStr"/>
+      <c r="V179" t="inlineStr"/>
+      <c r="W179" t="inlineStr"/>
+      <c r="X179" t="inlineStr"/>
+      <c r="Y179" t="inlineStr"/>
+      <c r="Z179" t="inlineStr"/>
+      <c r="AA179" t="inlineStr"/>
+      <c r="AB179" t="inlineStr"/>
+      <c r="AC179" t="inlineStr"/>
+      <c r="AD179" t="inlineStr"/>
+      <c r="AE179" t="inlineStr"/>
+      <c r="AF179" t="inlineStr"/>
+      <c r="AG179" t="inlineStr"/>
+      <c r="AH179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -15570,6 +18132,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U180" t="inlineStr"/>
+      <c r="V180" t="inlineStr"/>
+      <c r="W180" t="inlineStr"/>
+      <c r="X180" t="inlineStr"/>
+      <c r="Y180" t="inlineStr"/>
+      <c r="Z180" t="inlineStr"/>
+      <c r="AA180" t="inlineStr"/>
+      <c r="AB180" t="inlineStr"/>
+      <c r="AC180" t="inlineStr"/>
+      <c r="AD180" t="inlineStr"/>
+      <c r="AE180" t="inlineStr"/>
+      <c r="AF180" t="inlineStr"/>
+      <c r="AG180" t="inlineStr"/>
+      <c r="AH180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -15654,6 +18230,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U181" t="inlineStr"/>
+      <c r="V181" t="inlineStr"/>
+      <c r="W181" t="inlineStr"/>
+      <c r="X181" t="inlineStr"/>
+      <c r="Y181" t="inlineStr"/>
+      <c r="Z181" t="inlineStr"/>
+      <c r="AA181" t="inlineStr"/>
+      <c r="AB181" t="inlineStr"/>
+      <c r="AC181" t="inlineStr"/>
+      <c r="AD181" t="inlineStr"/>
+      <c r="AE181" t="inlineStr"/>
+      <c r="AF181" t="inlineStr"/>
+      <c r="AG181" t="inlineStr"/>
+      <c r="AH181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -15738,6 +18328,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U182" t="inlineStr"/>
+      <c r="V182" t="inlineStr"/>
+      <c r="W182" t="inlineStr"/>
+      <c r="X182" t="inlineStr"/>
+      <c r="Y182" t="inlineStr"/>
+      <c r="Z182" t="inlineStr"/>
+      <c r="AA182" t="inlineStr"/>
+      <c r="AB182" t="inlineStr"/>
+      <c r="AC182" t="inlineStr"/>
+      <c r="AD182" t="inlineStr"/>
+      <c r="AE182" t="inlineStr"/>
+      <c r="AF182" t="inlineStr"/>
+      <c r="AG182" t="inlineStr"/>
+      <c r="AH182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -15822,6 +18426,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U183" t="inlineStr"/>
+      <c r="V183" t="inlineStr"/>
+      <c r="W183" t="inlineStr"/>
+      <c r="X183" t="inlineStr"/>
+      <c r="Y183" t="inlineStr"/>
+      <c r="Z183" t="inlineStr"/>
+      <c r="AA183" t="inlineStr"/>
+      <c r="AB183" t="inlineStr"/>
+      <c r="AC183" t="inlineStr"/>
+      <c r="AD183" t="inlineStr"/>
+      <c r="AE183" t="inlineStr"/>
+      <c r="AF183" t="inlineStr"/>
+      <c r="AG183" t="inlineStr"/>
+      <c r="AH183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -15906,6 +18524,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U184" t="inlineStr"/>
+      <c r="V184" t="inlineStr"/>
+      <c r="W184" t="inlineStr"/>
+      <c r="X184" t="inlineStr"/>
+      <c r="Y184" t="inlineStr"/>
+      <c r="Z184" t="inlineStr"/>
+      <c r="AA184" t="inlineStr"/>
+      <c r="AB184" t="inlineStr"/>
+      <c r="AC184" t="inlineStr"/>
+      <c r="AD184" t="inlineStr"/>
+      <c r="AE184" t="inlineStr"/>
+      <c r="AF184" t="inlineStr"/>
+      <c r="AG184" t="inlineStr"/>
+      <c r="AH184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -15990,6 +18622,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U185" t="inlineStr"/>
+      <c r="V185" t="inlineStr"/>
+      <c r="W185" t="inlineStr"/>
+      <c r="X185" t="inlineStr"/>
+      <c r="Y185" t="inlineStr"/>
+      <c r="Z185" t="inlineStr"/>
+      <c r="AA185" t="inlineStr"/>
+      <c r="AB185" t="inlineStr"/>
+      <c r="AC185" t="inlineStr"/>
+      <c r="AD185" t="inlineStr"/>
+      <c r="AE185" t="inlineStr"/>
+      <c r="AF185" t="inlineStr"/>
+      <c r="AG185" t="inlineStr"/>
+      <c r="AH185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -16074,6 +18720,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U186" t="inlineStr"/>
+      <c r="V186" t="inlineStr"/>
+      <c r="W186" t="inlineStr"/>
+      <c r="X186" t="inlineStr"/>
+      <c r="Y186" t="inlineStr"/>
+      <c r="Z186" t="inlineStr"/>
+      <c r="AA186" t="inlineStr"/>
+      <c r="AB186" t="inlineStr"/>
+      <c r="AC186" t="inlineStr"/>
+      <c r="AD186" t="inlineStr"/>
+      <c r="AE186" t="inlineStr"/>
+      <c r="AF186" t="inlineStr"/>
+      <c r="AG186" t="inlineStr"/>
+      <c r="AH186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -16158,6 +18818,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U187" t="inlineStr"/>
+      <c r="V187" t="inlineStr"/>
+      <c r="W187" t="inlineStr"/>
+      <c r="X187" t="inlineStr"/>
+      <c r="Y187" t="inlineStr"/>
+      <c r="Z187" t="inlineStr"/>
+      <c r="AA187" t="inlineStr"/>
+      <c r="AB187" t="inlineStr"/>
+      <c r="AC187" t="inlineStr"/>
+      <c r="AD187" t="inlineStr"/>
+      <c r="AE187" t="inlineStr"/>
+      <c r="AF187" t="inlineStr"/>
+      <c r="AG187" t="inlineStr"/>
+      <c r="AH187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -16242,6 +18916,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U188" t="inlineStr"/>
+      <c r="V188" t="inlineStr"/>
+      <c r="W188" t="inlineStr"/>
+      <c r="X188" t="inlineStr"/>
+      <c r="Y188" t="inlineStr"/>
+      <c r="Z188" t="inlineStr"/>
+      <c r="AA188" t="inlineStr"/>
+      <c r="AB188" t="inlineStr"/>
+      <c r="AC188" t="inlineStr"/>
+      <c r="AD188" t="inlineStr"/>
+      <c r="AE188" t="inlineStr"/>
+      <c r="AF188" t="inlineStr"/>
+      <c r="AG188" t="inlineStr"/>
+      <c r="AH188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -16326,6 +19014,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U189" t="inlineStr"/>
+      <c r="V189" t="inlineStr"/>
+      <c r="W189" t="inlineStr"/>
+      <c r="X189" t="inlineStr"/>
+      <c r="Y189" t="inlineStr"/>
+      <c r="Z189" t="inlineStr"/>
+      <c r="AA189" t="inlineStr"/>
+      <c r="AB189" t="inlineStr"/>
+      <c r="AC189" t="inlineStr"/>
+      <c r="AD189" t="inlineStr"/>
+      <c r="AE189" t="inlineStr"/>
+      <c r="AF189" t="inlineStr"/>
+      <c r="AG189" t="inlineStr"/>
+      <c r="AH189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -16410,6 +19112,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U190" t="inlineStr"/>
+      <c r="V190" t="inlineStr"/>
+      <c r="W190" t="inlineStr"/>
+      <c r="X190" t="inlineStr"/>
+      <c r="Y190" t="inlineStr"/>
+      <c r="Z190" t="inlineStr"/>
+      <c r="AA190" t="inlineStr"/>
+      <c r="AB190" t="inlineStr"/>
+      <c r="AC190" t="inlineStr"/>
+      <c r="AD190" t="inlineStr"/>
+      <c r="AE190" t="inlineStr"/>
+      <c r="AF190" t="inlineStr"/>
+      <c r="AG190" t="inlineStr"/>
+      <c r="AH190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -16494,6 +19210,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U191" t="inlineStr"/>
+      <c r="V191" t="inlineStr"/>
+      <c r="W191" t="inlineStr"/>
+      <c r="X191" t="inlineStr"/>
+      <c r="Y191" t="inlineStr"/>
+      <c r="Z191" t="inlineStr"/>
+      <c r="AA191" t="inlineStr"/>
+      <c r="AB191" t="inlineStr"/>
+      <c r="AC191" t="inlineStr"/>
+      <c r="AD191" t="inlineStr"/>
+      <c r="AE191" t="inlineStr"/>
+      <c r="AF191" t="inlineStr"/>
+      <c r="AG191" t="inlineStr"/>
+      <c r="AH191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -16578,6 +19308,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U192" t="inlineStr"/>
+      <c r="V192" t="inlineStr"/>
+      <c r="W192" t="inlineStr"/>
+      <c r="X192" t="inlineStr"/>
+      <c r="Y192" t="inlineStr"/>
+      <c r="Z192" t="inlineStr"/>
+      <c r="AA192" t="inlineStr"/>
+      <c r="AB192" t="inlineStr"/>
+      <c r="AC192" t="inlineStr"/>
+      <c r="AD192" t="inlineStr"/>
+      <c r="AE192" t="inlineStr"/>
+      <c r="AF192" t="inlineStr"/>
+      <c r="AG192" t="inlineStr"/>
+      <c r="AH192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -16662,6 +19406,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U193" t="inlineStr"/>
+      <c r="V193" t="inlineStr"/>
+      <c r="W193" t="inlineStr"/>
+      <c r="X193" t="inlineStr"/>
+      <c r="Y193" t="inlineStr"/>
+      <c r="Z193" t="inlineStr"/>
+      <c r="AA193" t="inlineStr"/>
+      <c r="AB193" t="inlineStr"/>
+      <c r="AC193" t="inlineStr"/>
+      <c r="AD193" t="inlineStr"/>
+      <c r="AE193" t="inlineStr"/>
+      <c r="AF193" t="inlineStr"/>
+      <c r="AG193" t="inlineStr"/>
+      <c r="AH193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -16746,6 +19504,20 @@
           <t>جيد، لكن يمكن تحسين القيادة بتقليل الفرملة الحادة</t>
         </is>
       </c>
+      <c r="U194" t="inlineStr"/>
+      <c r="V194" t="inlineStr"/>
+      <c r="W194" t="inlineStr"/>
+      <c r="X194" t="inlineStr"/>
+      <c r="Y194" t="inlineStr"/>
+      <c r="Z194" t="inlineStr"/>
+      <c r="AA194" t="inlineStr"/>
+      <c r="AB194" t="inlineStr"/>
+      <c r="AC194" t="inlineStr"/>
+      <c r="AD194" t="inlineStr"/>
+      <c r="AE194" t="inlineStr"/>
+      <c r="AF194" t="inlineStr"/>
+      <c r="AG194" t="inlineStr"/>
+      <c r="AH194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -16830,6 +19602,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U195" t="inlineStr"/>
+      <c r="V195" t="inlineStr"/>
+      <c r="W195" t="inlineStr"/>
+      <c r="X195" t="inlineStr"/>
+      <c r="Y195" t="inlineStr"/>
+      <c r="Z195" t="inlineStr"/>
+      <c r="AA195" t="inlineStr"/>
+      <c r="AB195" t="inlineStr"/>
+      <c r="AC195" t="inlineStr"/>
+      <c r="AD195" t="inlineStr"/>
+      <c r="AE195" t="inlineStr"/>
+      <c r="AF195" t="inlineStr"/>
+      <c r="AG195" t="inlineStr"/>
+      <c r="AH195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -16914,6 +19700,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U196" t="inlineStr"/>
+      <c r="V196" t="inlineStr"/>
+      <c r="W196" t="inlineStr"/>
+      <c r="X196" t="inlineStr"/>
+      <c r="Y196" t="inlineStr"/>
+      <c r="Z196" t="inlineStr"/>
+      <c r="AA196" t="inlineStr"/>
+      <c r="AB196" t="inlineStr"/>
+      <c r="AC196" t="inlineStr"/>
+      <c r="AD196" t="inlineStr"/>
+      <c r="AE196" t="inlineStr"/>
+      <c r="AF196" t="inlineStr"/>
+      <c r="AG196" t="inlineStr"/>
+      <c r="AH196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -16998,6 +19798,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U197" t="inlineStr"/>
+      <c r="V197" t="inlineStr"/>
+      <c r="W197" t="inlineStr"/>
+      <c r="X197" t="inlineStr"/>
+      <c r="Y197" t="inlineStr"/>
+      <c r="Z197" t="inlineStr"/>
+      <c r="AA197" t="inlineStr"/>
+      <c r="AB197" t="inlineStr"/>
+      <c r="AC197" t="inlineStr"/>
+      <c r="AD197" t="inlineStr"/>
+      <c r="AE197" t="inlineStr"/>
+      <c r="AF197" t="inlineStr"/>
+      <c r="AG197" t="inlineStr"/>
+      <c r="AH197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -17082,6 +19896,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U198" t="inlineStr"/>
+      <c r="V198" t="inlineStr"/>
+      <c r="W198" t="inlineStr"/>
+      <c r="X198" t="inlineStr"/>
+      <c r="Y198" t="inlineStr"/>
+      <c r="Z198" t="inlineStr"/>
+      <c r="AA198" t="inlineStr"/>
+      <c r="AB198" t="inlineStr"/>
+      <c r="AC198" t="inlineStr"/>
+      <c r="AD198" t="inlineStr"/>
+      <c r="AE198" t="inlineStr"/>
+      <c r="AF198" t="inlineStr"/>
+      <c r="AG198" t="inlineStr"/>
+      <c r="AH198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -17166,6 +19994,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U199" t="inlineStr"/>
+      <c r="V199" t="inlineStr"/>
+      <c r="W199" t="inlineStr"/>
+      <c r="X199" t="inlineStr"/>
+      <c r="Y199" t="inlineStr"/>
+      <c r="Z199" t="inlineStr"/>
+      <c r="AA199" t="inlineStr"/>
+      <c r="AB199" t="inlineStr"/>
+      <c r="AC199" t="inlineStr"/>
+      <c r="AD199" t="inlineStr"/>
+      <c r="AE199" t="inlineStr"/>
+      <c r="AF199" t="inlineStr"/>
+      <c r="AG199" t="inlineStr"/>
+      <c r="AH199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -17250,6 +20092,20 @@
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
       </c>
+      <c r="U200" t="inlineStr"/>
+      <c r="V200" t="inlineStr"/>
+      <c r="W200" t="inlineStr"/>
+      <c r="X200" t="inlineStr"/>
+      <c r="Y200" t="inlineStr"/>
+      <c r="Z200" t="inlineStr"/>
+      <c r="AA200" t="inlineStr"/>
+      <c r="AB200" t="inlineStr"/>
+      <c r="AC200" t="inlineStr"/>
+      <c r="AD200" t="inlineStr"/>
+      <c r="AE200" t="inlineStr"/>
+      <c r="AF200" t="inlineStr"/>
+      <c r="AG200" t="inlineStr"/>
+      <c r="AH200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -17333,6 +20189,464 @@
         <is>
           <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
         </is>
+      </c>
+      <c r="U201" t="inlineStr"/>
+      <c r="V201" t="inlineStr"/>
+      <c r="W201" t="inlineStr"/>
+      <c r="X201" t="inlineStr"/>
+      <c r="Y201" t="inlineStr"/>
+      <c r="Z201" t="inlineStr"/>
+      <c r="AA201" t="inlineStr"/>
+      <c r="AB201" t="inlineStr"/>
+      <c r="AC201" t="inlineStr"/>
+      <c r="AD201" t="inlineStr"/>
+      <c r="AE201" t="inlineStr"/>
+      <c r="AF201" t="inlineStr"/>
+      <c r="AG201" t="inlineStr"/>
+      <c r="AH201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>6c220ab9</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>7f7590dd</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>2025-12-11 19:33:09.632717</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>0</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>risky</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>خطر</t>
+        </is>
+      </c>
+      <c r="G202" t="n">
+        <v>92.40000000000001</v>
+      </c>
+      <c r="H202" t="n">
+        <v>154.82</v>
+      </c>
+      <c r="I202" t="n">
+        <v>236</v>
+      </c>
+      <c r="J202" t="n">
+        <v>137</v>
+      </c>
+      <c r="K202" t="n">
+        <v>11</v>
+      </c>
+      <c r="L202" t="n">
+        <v>12.87</v>
+      </c>
+      <c r="M202" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="N202" t="n">
+        <v>100</v>
+      </c>
+      <c r="O202" t="inlineStr">
+        <is>
+          <t>highway</t>
+        </is>
+      </c>
+      <c r="P202" t="inlineStr">
+        <is>
+          <t>distracted</t>
+        </is>
+      </c>
+      <c r="Q202" t="inlineStr">
+        <is>
+          <t>midday</t>
+        </is>
+      </c>
+      <c r="R202" t="inlineStr">
+        <is>
+          <t>clear</t>
+        </is>
+      </c>
+      <c r="S202" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="T202" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="U202" t="inlineStr">
+        <is>
+          <t>قراءة إرشادات السلامة</t>
+        </is>
+      </c>
+      <c r="V202" t="inlineStr">
+        <is>
+          <t>2025-12-12</t>
+        </is>
+      </c>
+      <c r="W202" t="n">
+        <v>7</v>
+      </c>
+      <c r="X202" t="inlineStr"/>
+      <c r="Y202" t="inlineStr"/>
+      <c r="Z202" t="inlineStr"/>
+      <c r="AA202" t="inlineStr"/>
+      <c r="AB202" t="inlineStr"/>
+      <c r="AC202" t="inlineStr"/>
+      <c r="AD202" t="inlineStr"/>
+      <c r="AE202" t="inlineStr"/>
+      <c r="AF202" t="inlineStr"/>
+      <c r="AG202" t="inlineStr"/>
+      <c r="AH202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>6c220ab9</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>7f7590dd</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>2025-12-11 19:33:09.632717</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>0</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>risky</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>خطر</t>
+        </is>
+      </c>
+      <c r="G203" t="n">
+        <v>92.40000000000001</v>
+      </c>
+      <c r="H203" t="n">
+        <v>154.82</v>
+      </c>
+      <c r="I203" t="n">
+        <v>236</v>
+      </c>
+      <c r="J203" t="n">
+        <v>137</v>
+      </c>
+      <c r="K203" t="n">
+        <v>11</v>
+      </c>
+      <c r="L203" t="n">
+        <v>12.87</v>
+      </c>
+      <c r="M203" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="N203" t="n">
+        <v>100</v>
+      </c>
+      <c r="O203" t="inlineStr">
+        <is>
+          <t>highway</t>
+        </is>
+      </c>
+      <c r="P203" t="inlineStr">
+        <is>
+          <t>distracted</t>
+        </is>
+      </c>
+      <c r="Q203" t="inlineStr">
+        <is>
+          <t>midday</t>
+        </is>
+      </c>
+      <c r="R203" t="inlineStr">
+        <is>
+          <t>clear</t>
+        </is>
+      </c>
+      <c r="S203" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="T203" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="U203" t="inlineStr">
+        <is>
+          <t>قراءة إرشادات السلامة</t>
+        </is>
+      </c>
+      <c r="V203" t="inlineStr">
+        <is>
+          <t>2025-12-12</t>
+        </is>
+      </c>
+      <c r="W203" t="n">
+        <v>7</v>
+      </c>
+      <c r="X203" t="inlineStr"/>
+      <c r="Y203" t="inlineStr"/>
+      <c r="Z203" t="inlineStr"/>
+      <c r="AA203" t="inlineStr"/>
+      <c r="AB203" t="inlineStr"/>
+      <c r="AC203" t="inlineStr"/>
+      <c r="AD203" t="inlineStr"/>
+      <c r="AE203" t="inlineStr"/>
+      <c r="AF203" t="inlineStr"/>
+      <c r="AG203" t="inlineStr"/>
+      <c r="AH203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>6c220ab9</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>7f7590dd</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>2025-12-11 19:33:09.632717</t>
+        </is>
+      </c>
+      <c r="D204" t="n">
+        <v>0</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>risky</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>خطر</t>
+        </is>
+      </c>
+      <c r="G204" t="n">
+        <v>92.40000000000001</v>
+      </c>
+      <c r="H204" t="n">
+        <v>154.82</v>
+      </c>
+      <c r="I204" t="n">
+        <v>236</v>
+      </c>
+      <c r="J204" t="n">
+        <v>137</v>
+      </c>
+      <c r="K204" t="n">
+        <v>11</v>
+      </c>
+      <c r="L204" t="n">
+        <v>12.87</v>
+      </c>
+      <c r="M204" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="N204" t="n">
+        <v>100</v>
+      </c>
+      <c r="O204" t="inlineStr">
+        <is>
+          <t>highway</t>
+        </is>
+      </c>
+      <c r="P204" t="inlineStr">
+        <is>
+          <t>distracted</t>
+        </is>
+      </c>
+      <c r="Q204" t="inlineStr">
+        <is>
+          <t>midday</t>
+        </is>
+      </c>
+      <c r="R204" t="inlineStr">
+        <is>
+          <t>clear</t>
+        </is>
+      </c>
+      <c r="S204" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="T204" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="U204" t="inlineStr">
+        <is>
+          <t>قراءة إرشادات السلامة</t>
+        </is>
+      </c>
+      <c r="V204" t="inlineStr">
+        <is>
+          <t>2025-12-12</t>
+        </is>
+      </c>
+      <c r="W204" t="n">
+        <v>7</v>
+      </c>
+      <c r="X204" t="inlineStr"/>
+      <c r="Y204" t="inlineStr"/>
+      <c r="Z204" t="inlineStr"/>
+      <c r="AA204" t="inlineStr"/>
+      <c r="AB204" t="inlineStr"/>
+      <c r="AC204" t="inlineStr"/>
+      <c r="AD204" t="inlineStr"/>
+      <c r="AE204" t="inlineStr"/>
+      <c r="AF204" t="inlineStr"/>
+      <c r="AG204" t="inlineStr"/>
+      <c r="AH204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>6c220ab9</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>2025-12-11 19:33:09.632717</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>70</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>risky</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>خطر</t>
+        </is>
+      </c>
+      <c r="G205" t="n">
+        <v>80</v>
+      </c>
+      <c r="H205" t="n">
+        <v>120</v>
+      </c>
+      <c r="I205" t="n">
+        <v>2</v>
+      </c>
+      <c r="J205" t="n">
+        <v>1</v>
+      </c>
+      <c r="K205" t="n">
+        <v>5</v>
+      </c>
+      <c r="L205" t="n">
+        <v>0</v>
+      </c>
+      <c r="M205" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="N205" t="n">
+        <v>100</v>
+      </c>
+      <c r="O205" t="inlineStr">
+        <is>
+          <t>highway</t>
+        </is>
+      </c>
+      <c r="P205" t="inlineStr">
+        <is>
+          <t>distracted</t>
+        </is>
+      </c>
+      <c r="Q205" t="n">
+        <v>2</v>
+      </c>
+      <c r="R205" t="inlineStr">
+        <is>
+          <t>clear</t>
+        </is>
+      </c>
+      <c r="S205" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="T205" t="inlineStr">
+        <is>
+          <t>يجب تحسين أسلوب القيادة فوراً - تجنب السرعة الزائدة والفرملة الحادة</t>
+        </is>
+      </c>
+      <c r="U205" t="inlineStr"/>
+      <c r="V205" t="inlineStr"/>
+      <c r="W205" t="inlineStr"/>
+      <c r="X205" t="inlineStr">
+        <is>
+          <t>أحمد محمد العتيبي</t>
+        </is>
+      </c>
+      <c r="Y205" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z205" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA205" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB205" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC205" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD205" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE205" t="n">
+        <v>60</v>
+      </c>
+      <c r="AF205" t="n">
+        <v>50</v>
+      </c>
+      <c r="AG205" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH205" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>